<commit_message>
Fixing PDF jar importing problems and create database in case of first use of the program
</commit_message>
<xml_diff>
--- a/src/assets/reports/report.xlsx
+++ b/src/assets/reports/report.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3230E466-8489-480F-8661-146439FAA4F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683BCD28-EAFC-4B75-8531-E950617802EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1132,7 +1132,7 @@
     <numFmt numFmtId="166" formatCode="#."/>
     <numFmt numFmtId="167" formatCode="m\o\n\th\ d\,\ yyyy"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1153,13 +1153,6 @@
     </font>
     <font>
       <sz val="7.5"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="162"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="162"/>
@@ -1198,22 +1191,8 @@
       <charset val="162"/>
     </font>
     <font>
-      <sz val="6"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="162"/>
-    </font>
-    <font>
       <b/>
       <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="162"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="162"/>
@@ -1284,6 +1263,19 @@
       <family val="2"/>
       <charset val="162"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1736,228 +1728,198 @@
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="19" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="0">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="0">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="0">
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="30">
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="30">
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1969,64 +1931,52 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2040,134 +1990,101 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -2334,22 +2251,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>83128</xdr:colOff>
+      <xdr:colOff>152404</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>90056</xdr:rowOff>
+      <xdr:rowOff>117759</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>277092</xdr:colOff>
+      <xdr:colOff>277098</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
+      <xdr:rowOff>228598</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectangle 1">
+        <xdr:cNvPr id="8" name="Rectangle 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47F71585-16B6-4C11-8DBD-F4C725653AA7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C304B518-5F5B-4E51-8052-59AD0F31D9A4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2357,8 +2274,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1738746" y="6192983"/>
-          <a:ext cx="193964" cy="138544"/>
+          <a:off x="1808022" y="6220686"/>
+          <a:ext cx="124694" cy="110839"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2397,22 +2314,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>387929</xdr:colOff>
+      <xdr:colOff>457206</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>90059</xdr:rowOff>
+      <xdr:rowOff>117762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>581893</xdr:colOff>
+      <xdr:colOff>581900</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>228603</xdr:rowOff>
+      <xdr:rowOff>228601</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Rectangle 5">
+        <xdr:cNvPr id="11" name="Rectangle 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA003738-9FD6-4123-8A7D-3C10A51EE71C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C97102CD-1443-4A35-8050-47848BC7C78A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2420,8 +2337,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4059384" y="6192986"/>
-          <a:ext cx="193964" cy="138544"/>
+          <a:off x="4128661" y="6220689"/>
+          <a:ext cx="124694" cy="110839"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2723,8 +2640,8 @@
   </sheetPr>
   <dimension ref="A1:AB429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="T46" sqref="T46"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21:AB21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2758,450 +2675,450 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="120"/>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="126" t="s">
+      <c r="A1" s="93"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="99" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="127"/>
-      <c r="J1" s="127"/>
-      <c r="K1" s="127"/>
-      <c r="L1" s="127"/>
-      <c r="M1" s="127"/>
-      <c r="N1" s="127"/>
-      <c r="O1" s="127"/>
-      <c r="P1" s="127"/>
-      <c r="Q1" s="127"/>
-      <c r="R1" s="127"/>
-      <c r="S1" s="127"/>
-      <c r="T1" s="127"/>
-      <c r="U1" s="127"/>
-      <c r="V1" s="127"/>
-      <c r="W1" s="127"/>
-      <c r="X1" s="127"/>
-      <c r="Y1" s="127"/>
-      <c r="Z1" s="127"/>
-      <c r="AA1" s="127"/>
-      <c r="AB1" s="128"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
+      <c r="M1" s="100"/>
+      <c r="N1" s="100"/>
+      <c r="O1" s="100"/>
+      <c r="P1" s="100"/>
+      <c r="Q1" s="100"/>
+      <c r="R1" s="100"/>
+      <c r="S1" s="100"/>
+      <c r="T1" s="100"/>
+      <c r="U1" s="100"/>
+      <c r="V1" s="100"/>
+      <c r="W1" s="100"/>
+      <c r="X1" s="100"/>
+      <c r="Y1" s="100"/>
+      <c r="Z1" s="100"/>
+      <c r="AA1" s="100"/>
+      <c r="AB1" s="101"/>
     </row>
     <row r="2" spans="1:28" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="123"/>
-      <c r="B2" s="124"/>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
-      <c r="E2" s="124"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="125"/>
-      <c r="H2" s="129" t="s">
+      <c r="A2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="102" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="130"/>
-      <c r="J2" s="130"/>
-      <c r="K2" s="130"/>
-      <c r="L2" s="130"/>
-      <c r="M2" s="130"/>
-      <c r="N2" s="130"/>
-      <c r="O2" s="130"/>
-      <c r="P2" s="130"/>
-      <c r="Q2" s="130"/>
-      <c r="R2" s="130"/>
-      <c r="S2" s="130"/>
-      <c r="T2" s="130"/>
-      <c r="U2" s="130"/>
-      <c r="V2" s="130"/>
-      <c r="W2" s="130"/>
-      <c r="X2" s="130"/>
-      <c r="Y2" s="130"/>
-      <c r="Z2" s="130"/>
-      <c r="AA2" s="130"/>
-      <c r="AB2" s="131"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
+      <c r="N2" s="103"/>
+      <c r="O2" s="103"/>
+      <c r="P2" s="103"/>
+      <c r="Q2" s="103"/>
+      <c r="R2" s="103"/>
+      <c r="S2" s="103"/>
+      <c r="T2" s="103"/>
+      <c r="U2" s="103"/>
+      <c r="V2" s="103"/>
+      <c r="W2" s="103"/>
+      <c r="X2" s="103"/>
+      <c r="Y2" s="103"/>
+      <c r="Z2" s="103"/>
+      <c r="AA2" s="103"/>
+      <c r="AB2" s="104"/>
     </row>
     <row r="3" spans="1:28" s="3" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="132" t="s">
+      <c r="A3" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="133"/>
-      <c r="C3" s="133"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135"/>
-      <c r="H3" s="135"/>
-      <c r="I3" s="135"/>
-      <c r="J3" s="135"/>
-      <c r="K3" s="135"/>
-      <c r="L3" s="135"/>
-      <c r="M3" s="135"/>
-      <c r="N3" s="135"/>
-      <c r="O3" s="135"/>
-      <c r="P3" s="135"/>
-      <c r="Q3" s="136" t="s">
+      <c r="B3" s="106"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="107"/>
+      <c r="H3" s="107"/>
+      <c r="I3" s="107"/>
+      <c r="J3" s="107"/>
+      <c r="K3" s="107"/>
+      <c r="L3" s="107"/>
+      <c r="M3" s="107"/>
+      <c r="N3" s="107"/>
+      <c r="O3" s="107"/>
+      <c r="P3" s="107"/>
+      <c r="Q3" s="106" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="133"/>
-      <c r="S3" s="133"/>
-      <c r="T3" s="137"/>
-      <c r="U3" s="137"/>
-      <c r="V3" s="137"/>
-      <c r="W3" s="137"/>
-      <c r="X3" s="136" t="s">
+      <c r="R3" s="106"/>
+      <c r="S3" s="106"/>
+      <c r="T3" s="107"/>
+      <c r="U3" s="107"/>
+      <c r="V3" s="107"/>
+      <c r="W3" s="107"/>
+      <c r="X3" s="106" t="s">
         <v>7</v>
       </c>
-      <c r="Y3" s="133"/>
-      <c r="Z3" s="133"/>
-      <c r="AA3" s="138"/>
-      <c r="AB3" s="139"/>
+      <c r="Y3" s="106"/>
+      <c r="Z3" s="106"/>
+      <c r="AA3" s="108"/>
+      <c r="AB3" s="109"/>
     </row>
     <row r="4" spans="1:28" s="3" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="112"/>
-      <c r="C4" s="112"/>
-      <c r="D4" s="113"/>
-      <c r="E4" s="113"/>
-      <c r="F4" s="113"/>
-      <c r="G4" s="113"/>
-      <c r="H4" s="113"/>
-      <c r="I4" s="113"/>
-      <c r="J4" s="113"/>
-      <c r="K4" s="113"/>
-      <c r="L4" s="113"/>
-      <c r="M4" s="113"/>
-      <c r="N4" s="113"/>
-      <c r="O4" s="113"/>
-      <c r="P4" s="113"/>
-      <c r="Q4" s="39" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="112"/>
-      <c r="S4" s="112"/>
-      <c r="T4" s="118"/>
-      <c r="U4" s="119"/>
-      <c r="V4" s="119"/>
-      <c r="W4" s="119"/>
-      <c r="X4" s="39" t="s">
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="27"/>
+      <c r="U4" s="27"/>
+      <c r="V4" s="27"/>
+      <c r="W4" s="27"/>
+      <c r="X4" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="Y4" s="112"/>
-      <c r="Z4" s="112"/>
-      <c r="AA4" s="115"/>
-      <c r="AB4" s="116"/>
+      <c r="Y4" s="36"/>
+      <c r="Z4" s="36"/>
+      <c r="AA4" s="28"/>
+      <c r="AB4" s="92"/>
     </row>
     <row r="5" spans="1:28" s="3" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="112"/>
-      <c r="C5" s="112"/>
-      <c r="D5" s="117"/>
-      <c r="E5" s="113"/>
-      <c r="F5" s="113"/>
-      <c r="G5" s="113"/>
-      <c r="H5" s="113"/>
-      <c r="I5" s="113"/>
-      <c r="J5" s="113"/>
-      <c r="K5" s="113"/>
-      <c r="L5" s="113"/>
-      <c r="M5" s="113"/>
-      <c r="N5" s="113"/>
-      <c r="O5" s="113"/>
-      <c r="P5" s="113"/>
-      <c r="Q5" s="39" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="R5" s="112"/>
-      <c r="S5" s="112"/>
-      <c r="T5" s="114"/>
-      <c r="U5" s="114"/>
-      <c r="V5" s="114"/>
-      <c r="W5" s="114"/>
-      <c r="X5" s="39" t="s">
+      <c r="R5" s="36"/>
+      <c r="S5" s="36"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="27"/>
+      <c r="W5" s="27"/>
+      <c r="X5" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="Y5" s="112"/>
-      <c r="Z5" s="112"/>
-      <c r="AA5" s="115"/>
-      <c r="AB5" s="116"/>
+      <c r="Y5" s="36"/>
+      <c r="Z5" s="36"/>
+      <c r="AA5" s="28"/>
+      <c r="AB5" s="92"/>
     </row>
     <row r="6" spans="1:28" s="3" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="112"/>
-      <c r="C6" s="112"/>
-      <c r="D6" s="113"/>
-      <c r="E6" s="113"/>
-      <c r="F6" s="113"/>
-      <c r="G6" s="113"/>
-      <c r="H6" s="113"/>
-      <c r="I6" s="113"/>
-      <c r="J6" s="113"/>
-      <c r="K6" s="113"/>
-      <c r="L6" s="113"/>
-      <c r="M6" s="113"/>
-      <c r="N6" s="113"/>
-      <c r="O6" s="113"/>
-      <c r="P6" s="113"/>
-      <c r="Q6" s="39" t="s">
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="54"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="R6" s="112"/>
-      <c r="S6" s="112"/>
-      <c r="T6" s="114"/>
-      <c r="U6" s="114"/>
-      <c r="V6" s="114"/>
-      <c r="W6" s="114"/>
-      <c r="X6" s="39" t="s">
+      <c r="R6" s="36"/>
+      <c r="S6" s="36"/>
+      <c r="T6" s="27"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="27"/>
+      <c r="W6" s="27"/>
+      <c r="X6" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="Y6" s="112"/>
-      <c r="Z6" s="112"/>
-      <c r="AA6" s="115"/>
-      <c r="AB6" s="116"/>
+      <c r="Y6" s="36"/>
+      <c r="Z6" s="36"/>
+      <c r="AA6" s="28"/>
+      <c r="AB6" s="92"/>
     </row>
     <row r="7" spans="1:28" s="3" customFormat="1" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="107"/>
-      <c r="C7" s="107"/>
-      <c r="D7" s="108"/>
-      <c r="E7" s="108"/>
-      <c r="F7" s="108"/>
-      <c r="G7" s="108"/>
-      <c r="H7" s="108"/>
-      <c r="I7" s="108"/>
-      <c r="J7" s="108"/>
-      <c r="K7" s="108"/>
-      <c r="L7" s="108"/>
-      <c r="M7" s="108"/>
-      <c r="N7" s="108"/>
-      <c r="O7" s="108"/>
-      <c r="P7" s="108"/>
-      <c r="Q7" s="35" t="s">
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="44"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="R7" s="107"/>
-      <c r="S7" s="107"/>
-      <c r="T7" s="109"/>
-      <c r="U7" s="109"/>
-      <c r="V7" s="109"/>
-      <c r="W7" s="109"/>
-      <c r="X7" s="35" t="s">
+      <c r="R7" s="32"/>
+      <c r="S7" s="32"/>
+      <c r="T7" s="44"/>
+      <c r="U7" s="44"/>
+      <c r="V7" s="44"/>
+      <c r="W7" s="44"/>
+      <c r="X7" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Y7" s="107"/>
-      <c r="Z7" s="107"/>
-      <c r="AA7" s="110"/>
-      <c r="AB7" s="111"/>
+      <c r="Y7" s="32"/>
+      <c r="Z7" s="32"/>
+      <c r="AA7" s="56"/>
+      <c r="AB7" s="91"/>
     </row>
     <row r="8" spans="1:28" s="3" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="104" t="s">
+      <c r="A8" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="105"/>
-      <c r="C8" s="105"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="105"/>
-      <c r="G8" s="105"/>
-      <c r="H8" s="105"/>
-      <c r="I8" s="105"/>
-      <c r="J8" s="105"/>
-      <c r="K8" s="105"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="105"/>
-      <c r="N8" s="105"/>
-      <c r="O8" s="105"/>
-      <c r="P8" s="105"/>
-      <c r="Q8" s="105"/>
-      <c r="R8" s="105"/>
-      <c r="S8" s="105"/>
-      <c r="T8" s="105"/>
-      <c r="U8" s="105"/>
-      <c r="V8" s="105"/>
-      <c r="W8" s="105"/>
-      <c r="X8" s="105"/>
-      <c r="Y8" s="105"/>
-      <c r="Z8" s="105"/>
-      <c r="AA8" s="105"/>
-      <c r="AB8" s="106"/>
+      <c r="B8" s="89"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="89"/>
+      <c r="H8" s="89"/>
+      <c r="I8" s="89"/>
+      <c r="J8" s="89"/>
+      <c r="K8" s="89"/>
+      <c r="L8" s="89"/>
+      <c r="M8" s="89"/>
+      <c r="N8" s="89"/>
+      <c r="O8" s="89"/>
+      <c r="P8" s="89"/>
+      <c r="Q8" s="89"/>
+      <c r="R8" s="89"/>
+      <c r="S8" s="89"/>
+      <c r="T8" s="89"/>
+      <c r="U8" s="89"/>
+      <c r="V8" s="89"/>
+      <c r="W8" s="89"/>
+      <c r="X8" s="89"/>
+      <c r="Y8" s="89"/>
+      <c r="Z8" s="89"/>
+      <c r="AA8" s="89"/>
+      <c r="AB8" s="90"/>
     </row>
     <row r="9" spans="1:28" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="39" t="s">
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="43"/>
-      <c r="R9" s="43"/>
-      <c r="S9" s="43"/>
-      <c r="T9" s="43"/>
-      <c r="U9" s="43"/>
-      <c r="V9" s="43"/>
-      <c r="W9" s="39" t="s">
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="36"/>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="37"/>
+      <c r="S9" s="37"/>
+      <c r="T9" s="37"/>
+      <c r="U9" s="37"/>
+      <c r="V9" s="37"/>
+      <c r="W9" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="X9" s="39"/>
-      <c r="Y9" s="39"/>
-      <c r="Z9" s="43"/>
-      <c r="AA9" s="43"/>
-      <c r="AB9" s="44"/>
+      <c r="X9" s="36"/>
+      <c r="Y9" s="36"/>
+      <c r="Z9" s="37"/>
+      <c r="AA9" s="37"/>
+      <c r="AB9" s="41"/>
     </row>
     <row r="10" spans="1:28" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="39" t="s">
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="43"/>
-      <c r="R10" s="43"/>
-      <c r="S10" s="43"/>
-      <c r="T10" s="43"/>
-      <c r="U10" s="43"/>
-      <c r="V10" s="43"/>
-      <c r="W10" s="42" t="s">
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="36"/>
+      <c r="Q10" s="37"/>
+      <c r="R10" s="37"/>
+      <c r="S10" s="37"/>
+      <c r="T10" s="37"/>
+      <c r="U10" s="37"/>
+      <c r="V10" s="37"/>
+      <c r="W10" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="X10" s="42"/>
-      <c r="Y10" s="42"/>
-      <c r="Z10" s="43"/>
-      <c r="AA10" s="43"/>
-      <c r="AB10" s="44"/>
+      <c r="X10" s="40"/>
+      <c r="Y10" s="40"/>
+      <c r="Z10" s="37"/>
+      <c r="AA10" s="37"/>
+      <c r="AB10" s="41"/>
     </row>
     <row r="11" spans="1:28" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="39" t="s">
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="39"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="43"/>
-      <c r="R11" s="43"/>
-      <c r="S11" s="43"/>
-      <c r="T11" s="43"/>
-      <c r="U11" s="43"/>
-      <c r="V11" s="43"/>
-      <c r="W11" s="42"/>
-      <c r="X11" s="42"/>
-      <c r="Y11" s="42"/>
-      <c r="Z11" s="43"/>
-      <c r="AA11" s="43"/>
-      <c r="AB11" s="44"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="36"/>
+      <c r="P11" s="36"/>
+      <c r="Q11" s="37"/>
+      <c r="R11" s="37"/>
+      <c r="S11" s="37"/>
+      <c r="T11" s="37"/>
+      <c r="U11" s="37"/>
+      <c r="V11" s="37"/>
+      <c r="W11" s="40"/>
+      <c r="X11" s="40"/>
+      <c r="Y11" s="40"/>
+      <c r="Z11" s="37"/>
+      <c r="AA11" s="37"/>
+      <c r="AB11" s="41"/>
     </row>
     <row r="12" spans="1:28" s="4" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="39" t="s">
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="32"/>
-      <c r="R12" s="32"/>
-      <c r="S12" s="32"/>
-      <c r="T12" s="32"/>
-      <c r="U12" s="32"/>
-      <c r="V12" s="32"/>
-      <c r="W12" s="39" t="s">
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="37"/>
+      <c r="T12" s="37"/>
+      <c r="U12" s="37"/>
+      <c r="V12" s="37"/>
+      <c r="W12" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="X12" s="39"/>
-      <c r="Y12" s="39"/>
-      <c r="Z12" s="31"/>
-      <c r="AA12" s="32"/>
-      <c r="AB12" s="33"/>
+      <c r="X12" s="36"/>
+      <c r="Y12" s="36"/>
+      <c r="Z12" s="26"/>
+      <c r="AA12" s="26"/>
+      <c r="AB12" s="30"/>
     </row>
     <row r="13" spans="1:28" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="39" t="s">
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="39"/>
-      <c r="O13" s="39"/>
-      <c r="P13" s="39"/>
-      <c r="Q13" s="43"/>
-      <c r="R13" s="43"/>
-      <c r="S13" s="43"/>
-      <c r="T13" s="43"/>
-      <c r="U13" s="43"/>
-      <c r="V13" s="43"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="37"/>
+      <c r="S13" s="37"/>
+      <c r="T13" s="37"/>
+      <c r="U13" s="37"/>
+      <c r="V13" s="37"/>
       <c r="W13" s="14" t="s">
         <v>63</v>
       </c>
@@ -3212,32 +3129,32 @@
       <c r="AB13" s="22"/>
     </row>
     <row r="14" spans="1:28" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="35" t="s">
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="37"/>
-      <c r="R14" s="37"/>
-      <c r="S14" s="37"/>
-      <c r="T14" s="37"/>
-      <c r="U14" s="37"/>
-      <c r="V14" s="37"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="34"/>
+      <c r="T14" s="34"/>
+      <c r="U14" s="34"/>
+      <c r="V14" s="34"/>
       <c r="W14" s="17" t="s">
         <v>64</v>
       </c>
@@ -3248,351 +3165,351 @@
       <c r="AB14" s="25"/>
     </row>
     <row r="15" spans="1:28" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="90"/>
-      <c r="B15" s="91"/>
-      <c r="C15" s="91"/>
-      <c r="D15" s="91"/>
-      <c r="E15" s="91"/>
-      <c r="F15" s="91"/>
-      <c r="G15" s="91"/>
-      <c r="H15" s="93"/>
-      <c r="I15" s="93"/>
-      <c r="J15" s="93"/>
-      <c r="K15" s="93"/>
-      <c r="L15" s="93"/>
-      <c r="M15" s="93"/>
-      <c r="N15" s="93"/>
-      <c r="O15" s="93"/>
-      <c r="P15" s="94"/>
-      <c r="Q15" s="101" t="s">
+      <c r="A15" s="75"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="79"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="79"/>
+      <c r="L15" s="79"/>
+      <c r="M15" s="79"/>
+      <c r="N15" s="79"/>
+      <c r="O15" s="79"/>
+      <c r="P15" s="80"/>
+      <c r="Q15" s="85" t="s">
         <v>55</v>
       </c>
-      <c r="R15" s="102"/>
-      <c r="S15" s="102"/>
-      <c r="T15" s="102"/>
-      <c r="U15" s="102"/>
-      <c r="V15" s="102"/>
-      <c r="W15" s="102"/>
-      <c r="X15" s="102"/>
-      <c r="Y15" s="102"/>
-      <c r="Z15" s="102"/>
-      <c r="AA15" s="102"/>
-      <c r="AB15" s="103"/>
+      <c r="R15" s="86"/>
+      <c r="S15" s="86"/>
+      <c r="T15" s="86"/>
+      <c r="U15" s="86"/>
+      <c r="V15" s="86"/>
+      <c r="W15" s="86"/>
+      <c r="X15" s="86"/>
+      <c r="Y15" s="86"/>
+      <c r="Z15" s="86"/>
+      <c r="AA15" s="86"/>
+      <c r="AB15" s="87"/>
     </row>
     <row r="16" spans="1:28" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="92"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="95"/>
-      <c r="I16" s="95"/>
-      <c r="J16" s="95"/>
-      <c r="K16" s="95"/>
-      <c r="L16" s="95"/>
-      <c r="M16" s="95"/>
-      <c r="N16" s="95"/>
-      <c r="O16" s="95"/>
-      <c r="P16" s="96"/>
-      <c r="Q16" s="97" t="s">
+      <c r="A16" s="77"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="81"/>
+      <c r="I16" s="81"/>
+      <c r="J16" s="81"/>
+      <c r="K16" s="81"/>
+      <c r="L16" s="81"/>
+      <c r="M16" s="81"/>
+      <c r="N16" s="81"/>
+      <c r="O16" s="81"/>
+      <c r="P16" s="82"/>
+      <c r="Q16" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="R16" s="98"/>
-      <c r="S16" s="84" t="s">
+      <c r="R16" s="84"/>
+      <c r="S16" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="T16" s="84"/>
-      <c r="U16" s="84"/>
-      <c r="V16" s="84"/>
-      <c r="W16" s="84"/>
-      <c r="X16" s="84"/>
-      <c r="Y16" s="84"/>
-      <c r="Z16" s="84"/>
-      <c r="AA16" s="84"/>
-      <c r="AB16" s="85"/>
+      <c r="T16" s="69"/>
+      <c r="U16" s="69"/>
+      <c r="V16" s="69"/>
+      <c r="W16" s="69"/>
+      <c r="X16" s="69"/>
+      <c r="Y16" s="69"/>
+      <c r="Z16" s="69"/>
+      <c r="AA16" s="69"/>
+      <c r="AB16" s="70"/>
     </row>
     <row r="17" spans="1:28" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="92"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="95"/>
-      <c r="I17" s="95"/>
-      <c r="J17" s="95"/>
-      <c r="K17" s="95"/>
-      <c r="L17" s="95"/>
-      <c r="M17" s="95"/>
-      <c r="N17" s="95"/>
-      <c r="O17" s="95"/>
-      <c r="P17" s="96"/>
-      <c r="Q17" s="99" t="s">
+      <c r="A17" s="77"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="81"/>
+      <c r="I17" s="81"/>
+      <c r="J17" s="81"/>
+      <c r="K17" s="81"/>
+      <c r="L17" s="81"/>
+      <c r="M17" s="81"/>
+      <c r="N17" s="81"/>
+      <c r="O17" s="81"/>
+      <c r="P17" s="82"/>
+      <c r="Q17" s="83" t="s">
         <v>61</v>
       </c>
-      <c r="R17" s="98"/>
-      <c r="S17" s="100" t="s">
+      <c r="R17" s="84"/>
+      <c r="S17" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="T17" s="84"/>
-      <c r="U17" s="84"/>
-      <c r="V17" s="84"/>
-      <c r="W17" s="84"/>
-      <c r="X17" s="84"/>
-      <c r="Y17" s="84"/>
-      <c r="Z17" s="84"/>
-      <c r="AA17" s="84"/>
-      <c r="AB17" s="85"/>
+      <c r="T17" s="69"/>
+      <c r="U17" s="69"/>
+      <c r="V17" s="69"/>
+      <c r="W17" s="69"/>
+      <c r="X17" s="69"/>
+      <c r="Y17" s="69"/>
+      <c r="Z17" s="69"/>
+      <c r="AA17" s="69"/>
+      <c r="AB17" s="70"/>
     </row>
     <row r="18" spans="1:28" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="92"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="95"/>
-      <c r="I18" s="95"/>
-      <c r="J18" s="95"/>
-      <c r="K18" s="95"/>
-      <c r="L18" s="95"/>
-      <c r="M18" s="95"/>
-      <c r="N18" s="95"/>
-      <c r="O18" s="95"/>
-      <c r="P18" s="96"/>
-      <c r="Q18" s="99" t="s">
+      <c r="A18" s="77"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="78"/>
+      <c r="H18" s="81"/>
+      <c r="I18" s="81"/>
+      <c r="J18" s="81"/>
+      <c r="K18" s="81"/>
+      <c r="L18" s="81"/>
+      <c r="M18" s="81"/>
+      <c r="N18" s="81"/>
+      <c r="O18" s="81"/>
+      <c r="P18" s="82"/>
+      <c r="Q18" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="R18" s="98"/>
-      <c r="S18" s="84" t="s">
+      <c r="R18" s="84"/>
+      <c r="S18" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="T18" s="84"/>
-      <c r="U18" s="84"/>
-      <c r="V18" s="84"/>
-      <c r="W18" s="84"/>
-      <c r="X18" s="84"/>
-      <c r="Y18" s="84"/>
-      <c r="Z18" s="84"/>
-      <c r="AA18" s="84"/>
-      <c r="AB18" s="85"/>
+      <c r="T18" s="69"/>
+      <c r="U18" s="69"/>
+      <c r="V18" s="69"/>
+      <c r="W18" s="69"/>
+      <c r="X18" s="69"/>
+      <c r="Y18" s="69"/>
+      <c r="Z18" s="69"/>
+      <c r="AA18" s="69"/>
+      <c r="AB18" s="70"/>
     </row>
     <row r="19" spans="1:28" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="92"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="95"/>
-      <c r="I19" s="95"/>
-      <c r="J19" s="95"/>
-      <c r="K19" s="95"/>
-      <c r="L19" s="95"/>
-      <c r="M19" s="95"/>
-      <c r="N19" s="95"/>
-      <c r="O19" s="95"/>
-      <c r="P19" s="96"/>
-      <c r="Q19" s="86" t="s">
+      <c r="A19" s="77"/>
+      <c r="B19" s="78"/>
+      <c r="C19" s="78"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="81"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="81"/>
+      <c r="L19" s="81"/>
+      <c r="M19" s="81"/>
+      <c r="N19" s="81"/>
+      <c r="O19" s="81"/>
+      <c r="P19" s="82"/>
+      <c r="Q19" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="R19" s="87"/>
-      <c r="S19" s="88" t="s">
+      <c r="R19" s="72"/>
+      <c r="S19" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="T19" s="88"/>
-      <c r="U19" s="88"/>
-      <c r="V19" s="88"/>
-      <c r="W19" s="88"/>
-      <c r="X19" s="88"/>
-      <c r="Y19" s="88"/>
-      <c r="Z19" s="88"/>
-      <c r="AA19" s="88"/>
-      <c r="AB19" s="89"/>
+      <c r="T19" s="73"/>
+      <c r="U19" s="73"/>
+      <c r="V19" s="73"/>
+      <c r="W19" s="73"/>
+      <c r="X19" s="73"/>
+      <c r="Y19" s="73"/>
+      <c r="Z19" s="73"/>
+      <c r="AA19" s="73"/>
+      <c r="AB19" s="74"/>
     </row>
     <row r="20" spans="1:28" ht="26.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="72" t="s">
+      <c r="A20" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="73"/>
-      <c r="C20" s="73"/>
-      <c r="D20" s="73"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="73"/>
-      <c r="G20" s="73"/>
-      <c r="H20" s="74"/>
-      <c r="I20" s="74"/>
-      <c r="J20" s="74"/>
-      <c r="K20" s="74"/>
-      <c r="L20" s="74"/>
-      <c r="M20" s="74"/>
-      <c r="N20" s="74"/>
-      <c r="O20" s="74"/>
-      <c r="P20" s="74"/>
-      <c r="Q20" s="75"/>
-      <c r="R20" s="75"/>
-      <c r="S20" s="75"/>
-      <c r="T20" s="75"/>
-      <c r="U20" s="75"/>
-      <c r="V20" s="75"/>
-      <c r="W20" s="75"/>
-      <c r="X20" s="75"/>
-      <c r="Y20" s="75"/>
-      <c r="Z20" s="75"/>
-      <c r="AA20" s="75"/>
-      <c r="AB20" s="76"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="110"/>
+      <c r="I20" s="110"/>
+      <c r="J20" s="110"/>
+      <c r="K20" s="110"/>
+      <c r="L20" s="110"/>
+      <c r="M20" s="110"/>
+      <c r="N20" s="110"/>
+      <c r="O20" s="110"/>
+      <c r="P20" s="110"/>
+      <c r="Q20" s="111"/>
+      <c r="R20" s="111"/>
+      <c r="S20" s="111"/>
+      <c r="T20" s="111"/>
+      <c r="U20" s="111"/>
+      <c r="V20" s="111"/>
+      <c r="W20" s="111"/>
+      <c r="X20" s="111"/>
+      <c r="Y20" s="111"/>
+      <c r="Z20" s="111"/>
+      <c r="AA20" s="111"/>
+      <c r="AB20" s="112"/>
     </row>
     <row r="21" spans="1:28" ht="26.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="77" t="s">
+      <c r="A21" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="78"/>
-      <c r="C21" s="78"/>
-      <c r="D21" s="78"/>
-      <c r="E21" s="78"/>
-      <c r="F21" s="78"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="79"/>
-      <c r="I21" s="79"/>
-      <c r="J21" s="79"/>
-      <c r="K21" s="79"/>
-      <c r="L21" s="79"/>
-      <c r="M21" s="79"/>
-      <c r="N21" s="79"/>
-      <c r="O21" s="79"/>
-      <c r="P21" s="79"/>
-      <c r="Q21" s="79"/>
-      <c r="R21" s="79"/>
-      <c r="S21" s="79"/>
-      <c r="T21" s="79"/>
-      <c r="U21" s="79"/>
-      <c r="V21" s="79"/>
-      <c r="W21" s="79"/>
-      <c r="X21" s="79"/>
-      <c r="Y21" s="79"/>
-      <c r="Z21" s="79"/>
-      <c r="AA21" s="79"/>
-      <c r="AB21" s="80"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="113"/>
+      <c r="I21" s="113"/>
+      <c r="J21" s="113"/>
+      <c r="K21" s="113"/>
+      <c r="L21" s="113"/>
+      <c r="M21" s="113"/>
+      <c r="N21" s="113"/>
+      <c r="O21" s="113"/>
+      <c r="P21" s="113"/>
+      <c r="Q21" s="113"/>
+      <c r="R21" s="113"/>
+      <c r="S21" s="113"/>
+      <c r="T21" s="113"/>
+      <c r="U21" s="113"/>
+      <c r="V21" s="113"/>
+      <c r="W21" s="113"/>
+      <c r="X21" s="113"/>
+      <c r="Y21" s="113"/>
+      <c r="Z21" s="113"/>
+      <c r="AA21" s="113"/>
+      <c r="AB21" s="114"/>
     </row>
     <row r="22" spans="1:28" ht="26.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="81" t="s">
+      <c r="A22" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="82"/>
-      <c r="C22" s="82"/>
-      <c r="D22" s="82"/>
-      <c r="E22" s="82"/>
-      <c r="F22" s="82"/>
-      <c r="G22" s="82"/>
-      <c r="H22" s="66"/>
-      <c r="I22" s="66"/>
-      <c r="J22" s="66"/>
-      <c r="K22" s="66"/>
-      <c r="L22" s="66"/>
-      <c r="M22" s="66"/>
-      <c r="N22" s="66"/>
-      <c r="O22" s="66"/>
-      <c r="P22" s="66"/>
-      <c r="Q22" s="66"/>
-      <c r="R22" s="66"/>
-      <c r="S22" s="66"/>
-      <c r="T22" s="66"/>
-      <c r="U22" s="66"/>
-      <c r="V22" s="66"/>
-      <c r="W22" s="66"/>
-      <c r="X22" s="66"/>
-      <c r="Y22" s="66"/>
-      <c r="Z22" s="66"/>
-      <c r="AA22" s="66"/>
-      <c r="AB22" s="83"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="55"/>
+      <c r="J22" s="55"/>
+      <c r="K22" s="55"/>
+      <c r="L22" s="55"/>
+      <c r="M22" s="55"/>
+      <c r="N22" s="55"/>
+      <c r="O22" s="55"/>
+      <c r="P22" s="55"/>
+      <c r="Q22" s="55"/>
+      <c r="R22" s="55"/>
+      <c r="S22" s="55"/>
+      <c r="T22" s="55"/>
+      <c r="U22" s="55"/>
+      <c r="V22" s="55"/>
+      <c r="W22" s="55"/>
+      <c r="X22" s="55"/>
+      <c r="Y22" s="55"/>
+      <c r="Z22" s="55"/>
+      <c r="AA22" s="55"/>
+      <c r="AB22" s="68"/>
     </row>
     <row r="23" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="67" t="s">
+      <c r="A23" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="57"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="57"/>
-      <c r="J23" s="57"/>
-      <c r="K23" s="57"/>
-      <c r="L23" s="57"/>
-      <c r="M23" s="57"/>
-      <c r="N23" s="57"/>
-      <c r="O23" s="57"/>
-      <c r="P23" s="57"/>
-      <c r="Q23" s="57"/>
-      <c r="R23" s="57"/>
-      <c r="S23" s="57"/>
-      <c r="T23" s="57"/>
-      <c r="U23" s="57"/>
-      <c r="V23" s="57"/>
-      <c r="W23" s="57"/>
-      <c r="X23" s="57"/>
-      <c r="Y23" s="57"/>
-      <c r="Z23" s="57"/>
-      <c r="AA23" s="57"/>
-      <c r="AB23" s="58"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="52"/>
+      <c r="N23" s="52"/>
+      <c r="O23" s="52"/>
+      <c r="P23" s="52"/>
+      <c r="Q23" s="52"/>
+      <c r="R23" s="52"/>
+      <c r="S23" s="52"/>
+      <c r="T23" s="52"/>
+      <c r="U23" s="52"/>
+      <c r="V23" s="52"/>
+      <c r="W23" s="52"/>
+      <c r="X23" s="52"/>
+      <c r="Y23" s="52"/>
+      <c r="Z23" s="52"/>
+      <c r="AA23" s="52"/>
+      <c r="AB23" s="53"/>
     </row>
     <row r="24" spans="1:28" s="3" customFormat="1" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="68" t="s">
+      <c r="B24" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="69"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="69"/>
-      <c r="G24" s="69"/>
-      <c r="H24" s="69"/>
-      <c r="I24" s="68" t="s">
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="J24" s="68"/>
-      <c r="K24" s="68"/>
-      <c r="L24" s="42" t="s">
+      <c r="J24" s="59"/>
+      <c r="K24" s="59"/>
+      <c r="L24" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="M24" s="42"/>
-      <c r="N24" s="42"/>
-      <c r="O24" s="42"/>
-      <c r="P24" s="42"/>
-      <c r="Q24" s="42"/>
-      <c r="R24" s="11" t="s">
+      <c r="M24" s="40"/>
+      <c r="N24" s="40"/>
+      <c r="O24" s="40"/>
+      <c r="P24" s="40"/>
+      <c r="Q24" s="40"/>
+      <c r="R24" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="S24" s="68" t="s">
+      <c r="S24" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="T24" s="68"/>
-      <c r="U24" s="68"/>
-      <c r="V24" s="68"/>
-      <c r="W24" s="70" t="s">
+      <c r="T24" s="59"/>
+      <c r="U24" s="59"/>
+      <c r="V24" s="59"/>
+      <c r="W24" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="X24" s="71"/>
-      <c r="Y24" s="68" t="s">
+      <c r="X24" s="61"/>
+      <c r="Y24" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="Z24" s="69"/>
-      <c r="AA24" s="69"/>
+      <c r="Z24" s="59"/>
+      <c r="AA24" s="59"/>
       <c r="AB24" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
+      <c r="A25" s="9">
         <v>1</v>
       </c>
       <c r="B25" s="26"/>
@@ -3611,20 +3528,20 @@
       <c r="O25" s="27"/>
       <c r="P25" s="27"/>
       <c r="Q25" s="27"/>
-      <c r="R25" s="12"/>
+      <c r="R25" s="8"/>
       <c r="S25" s="27"/>
       <c r="T25" s="27"/>
       <c r="U25" s="27"/>
       <c r="V25" s="27"/>
       <c r="W25" s="28"/>
       <c r="X25" s="29"/>
-      <c r="Y25" s="30"/>
-      <c r="Z25" s="30"/>
-      <c r="AA25" s="30"/>
-      <c r="AB25" s="8"/>
+      <c r="Y25" s="26"/>
+      <c r="Z25" s="26"/>
+      <c r="AA25" s="26"/>
+      <c r="AB25" s="10"/>
     </row>
     <row r="26" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
+      <c r="A26" s="9">
         <v>2</v>
       </c>
       <c r="B26" s="26"/>
@@ -3643,20 +3560,20 @@
       <c r="O26" s="27"/>
       <c r="P26" s="27"/>
       <c r="Q26" s="27"/>
-      <c r="R26" s="12"/>
+      <c r="R26" s="8"/>
       <c r="S26" s="27"/>
       <c r="T26" s="27"/>
       <c r="U26" s="27"/>
       <c r="V26" s="27"/>
       <c r="W26" s="28"/>
       <c r="X26" s="29"/>
-      <c r="Y26" s="30"/>
-      <c r="Z26" s="30"/>
-      <c r="AA26" s="30"/>
-      <c r="AB26" s="8"/>
+      <c r="Y26" s="26"/>
+      <c r="Z26" s="26"/>
+      <c r="AA26" s="26"/>
+      <c r="AB26" s="10"/>
     </row>
     <row r="27" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
+      <c r="A27" s="9">
         <v>3</v>
       </c>
       <c r="B27" s="26"/>
@@ -3675,20 +3592,20 @@
       <c r="O27" s="27"/>
       <c r="P27" s="27"/>
       <c r="Q27" s="27"/>
-      <c r="R27" s="12"/>
+      <c r="R27" s="8"/>
       <c r="S27" s="27"/>
       <c r="T27" s="27"/>
       <c r="U27" s="27"/>
       <c r="V27" s="27"/>
       <c r="W27" s="28"/>
       <c r="X27" s="29"/>
-      <c r="Y27" s="30"/>
-      <c r="Z27" s="30"/>
-      <c r="AA27" s="30"/>
-      <c r="AB27" s="8"/>
+      <c r="Y27" s="26"/>
+      <c r="Z27" s="26"/>
+      <c r="AA27" s="26"/>
+      <c r="AB27" s="10"/>
     </row>
     <row r="28" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7">
+      <c r="A28" s="9">
         <v>4</v>
       </c>
       <c r="B28" s="26"/>
@@ -3707,20 +3624,20 @@
       <c r="O28" s="27"/>
       <c r="P28" s="27"/>
       <c r="Q28" s="27"/>
-      <c r="R28" s="12"/>
+      <c r="R28" s="8"/>
       <c r="S28" s="27"/>
       <c r="T28" s="27"/>
       <c r="U28" s="27"/>
       <c r="V28" s="27"/>
       <c r="W28" s="28"/>
       <c r="X28" s="29"/>
-      <c r="Y28" s="30"/>
-      <c r="Z28" s="30"/>
-      <c r="AA28" s="30"/>
-      <c r="AB28" s="8"/>
+      <c r="Y28" s="26"/>
+      <c r="Z28" s="26"/>
+      <c r="AA28" s="26"/>
+      <c r="AB28" s="10"/>
     </row>
     <row r="29" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
+      <c r="A29" s="9">
         <v>5</v>
       </c>
       <c r="B29" s="26"/>
@@ -3739,20 +3656,20 @@
       <c r="O29" s="27"/>
       <c r="P29" s="27"/>
       <c r="Q29" s="27"/>
-      <c r="R29" s="12"/>
+      <c r="R29" s="8"/>
       <c r="S29" s="27"/>
       <c r="T29" s="27"/>
       <c r="U29" s="27"/>
       <c r="V29" s="27"/>
       <c r="W29" s="28"/>
       <c r="X29" s="29"/>
-      <c r="Y29" s="30"/>
-      <c r="Z29" s="30"/>
-      <c r="AA29" s="30"/>
-      <c r="AB29" s="8"/>
+      <c r="Y29" s="26"/>
+      <c r="Z29" s="26"/>
+      <c r="AA29" s="26"/>
+      <c r="AB29" s="10"/>
     </row>
     <row r="30" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
+      <c r="A30" s="9">
         <v>6</v>
       </c>
       <c r="B30" s="26"/>
@@ -3771,20 +3688,20 @@
       <c r="O30" s="27"/>
       <c r="P30" s="27"/>
       <c r="Q30" s="27"/>
-      <c r="R30" s="12"/>
+      <c r="R30" s="8"/>
       <c r="S30" s="27"/>
       <c r="T30" s="27"/>
       <c r="U30" s="27"/>
       <c r="V30" s="27"/>
       <c r="W30" s="28"/>
       <c r="X30" s="29"/>
-      <c r="Y30" s="30"/>
-      <c r="Z30" s="30"/>
-      <c r="AA30" s="30"/>
-      <c r="AB30" s="8"/>
+      <c r="Y30" s="26"/>
+      <c r="Z30" s="26"/>
+      <c r="AA30" s="26"/>
+      <c r="AB30" s="10"/>
     </row>
     <row r="31" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="7">
+      <c r="A31" s="9">
         <v>7</v>
       </c>
       <c r="B31" s="26"/>
@@ -3803,20 +3720,20 @@
       <c r="O31" s="27"/>
       <c r="P31" s="27"/>
       <c r="Q31" s="27"/>
-      <c r="R31" s="12"/>
+      <c r="R31" s="8"/>
       <c r="S31" s="27"/>
       <c r="T31" s="27"/>
       <c r="U31" s="27"/>
       <c r="V31" s="27"/>
       <c r="W31" s="28"/>
       <c r="X31" s="29"/>
-      <c r="Y31" s="30"/>
-      <c r="Z31" s="30"/>
-      <c r="AA31" s="30"/>
-      <c r="AB31" s="8"/>
+      <c r="Y31" s="26"/>
+      <c r="Z31" s="26"/>
+      <c r="AA31" s="26"/>
+      <c r="AB31" s="10"/>
     </row>
     <row r="32" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7">
+      <c r="A32" s="9">
         <v>8</v>
       </c>
       <c r="B32" s="26"/>
@@ -3835,20 +3752,20 @@
       <c r="O32" s="27"/>
       <c r="P32" s="27"/>
       <c r="Q32" s="27"/>
-      <c r="R32" s="12"/>
+      <c r="R32" s="8"/>
       <c r="S32" s="27"/>
       <c r="T32" s="27"/>
       <c r="U32" s="27"/>
       <c r="V32" s="27"/>
       <c r="W32" s="28"/>
       <c r="X32" s="29"/>
-      <c r="Y32" s="30"/>
-      <c r="Z32" s="30"/>
-      <c r="AA32" s="30"/>
-      <c r="AB32" s="8"/>
+      <c r="Y32" s="26"/>
+      <c r="Z32" s="26"/>
+      <c r="AA32" s="26"/>
+      <c r="AB32" s="10"/>
     </row>
     <row r="33" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7">
+      <c r="A33" s="9">
         <v>9</v>
       </c>
       <c r="B33" s="26"/>
@@ -3867,20 +3784,20 @@
       <c r="O33" s="27"/>
       <c r="P33" s="27"/>
       <c r="Q33" s="27"/>
-      <c r="R33" s="12"/>
+      <c r="R33" s="8"/>
       <c r="S33" s="27"/>
       <c r="T33" s="27"/>
       <c r="U33" s="27"/>
       <c r="V33" s="27"/>
       <c r="W33" s="28"/>
       <c r="X33" s="29"/>
-      <c r="Y33" s="30"/>
-      <c r="Z33" s="30"/>
-      <c r="AA33" s="30"/>
-      <c r="AB33" s="8"/>
+      <c r="Y33" s="26"/>
+      <c r="Z33" s="26"/>
+      <c r="AA33" s="26"/>
+      <c r="AB33" s="10"/>
     </row>
     <row r="34" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7">
+      <c r="A34" s="9">
         <v>10</v>
       </c>
       <c r="B34" s="26"/>
@@ -3899,20 +3816,20 @@
       <c r="O34" s="27"/>
       <c r="P34" s="27"/>
       <c r="Q34" s="27"/>
-      <c r="R34" s="12"/>
+      <c r="R34" s="8"/>
       <c r="S34" s="27"/>
       <c r="T34" s="27"/>
       <c r="U34" s="27"/>
       <c r="V34" s="27"/>
       <c r="W34" s="28"/>
       <c r="X34" s="29"/>
-      <c r="Y34" s="30"/>
-      <c r="Z34" s="30"/>
-      <c r="AA34" s="30"/>
-      <c r="AB34" s="8"/>
+      <c r="Y34" s="26"/>
+      <c r="Z34" s="26"/>
+      <c r="AA34" s="26"/>
+      <c r="AB34" s="10"/>
     </row>
     <row r="35" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="7">
+      <c r="A35" s="9">
         <v>11</v>
       </c>
       <c r="B35" s="26"/>
@@ -3931,20 +3848,20 @@
       <c r="O35" s="27"/>
       <c r="P35" s="27"/>
       <c r="Q35" s="27"/>
-      <c r="R35" s="12"/>
+      <c r="R35" s="8"/>
       <c r="S35" s="27"/>
       <c r="T35" s="27"/>
       <c r="U35" s="27"/>
       <c r="V35" s="27"/>
       <c r="W35" s="28"/>
       <c r="X35" s="29"/>
-      <c r="Y35" s="30"/>
-      <c r="Z35" s="30"/>
-      <c r="AA35" s="30"/>
-      <c r="AB35" s="8"/>
+      <c r="Y35" s="26"/>
+      <c r="Z35" s="26"/>
+      <c r="AA35" s="26"/>
+      <c r="AB35" s="10"/>
     </row>
     <row r="36" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="7">
+      <c r="A36" s="9">
         <v>12</v>
       </c>
       <c r="B36" s="26"/>
@@ -3963,20 +3880,20 @@
       <c r="O36" s="27"/>
       <c r="P36" s="27"/>
       <c r="Q36" s="27"/>
-      <c r="R36" s="12"/>
+      <c r="R36" s="8"/>
       <c r="S36" s="27"/>
       <c r="T36" s="27"/>
       <c r="U36" s="27"/>
       <c r="V36" s="27"/>
       <c r="W36" s="28"/>
       <c r="X36" s="29"/>
-      <c r="Y36" s="30"/>
-      <c r="Z36" s="30"/>
-      <c r="AA36" s="30"/>
-      <c r="AB36" s="8"/>
+      <c r="Y36" s="26"/>
+      <c r="Z36" s="26"/>
+      <c r="AA36" s="26"/>
+      <c r="AB36" s="10"/>
     </row>
     <row r="37" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="7">
+      <c r="A37" s="9">
         <v>13</v>
       </c>
       <c r="B37" s="26"/>
@@ -3995,249 +3912,249 @@
       <c r="O37" s="27"/>
       <c r="P37" s="27"/>
       <c r="Q37" s="27"/>
-      <c r="R37" s="12"/>
+      <c r="R37" s="8"/>
       <c r="S37" s="27"/>
       <c r="T37" s="27"/>
       <c r="U37" s="27"/>
       <c r="V37" s="27"/>
       <c r="W37" s="28"/>
       <c r="X37" s="29"/>
-      <c r="Y37" s="30"/>
-      <c r="Z37" s="30"/>
-      <c r="AA37" s="30"/>
-      <c r="AB37" s="8"/>
+      <c r="Y37" s="26"/>
+      <c r="Z37" s="26"/>
+      <c r="AA37" s="26"/>
+      <c r="AB37" s="10"/>
     </row>
     <row r="38" spans="1:28" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="9">
+      <c r="A38" s="11">
         <v>14</v>
       </c>
-      <c r="B38" s="62"/>
-      <c r="C38" s="62"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="62"/>
-      <c r="F38" s="62"/>
-      <c r="G38" s="62"/>
-      <c r="H38" s="62"/>
-      <c r="I38" s="63"/>
-      <c r="J38" s="63"/>
-      <c r="K38" s="63"/>
-      <c r="L38" s="63"/>
-      <c r="M38" s="63"/>
-      <c r="N38" s="63"/>
-      <c r="O38" s="63"/>
-      <c r="P38" s="63"/>
-      <c r="Q38" s="63"/>
-      <c r="R38" s="13"/>
-      <c r="S38" s="63"/>
-      <c r="T38" s="63"/>
-      <c r="U38" s="63"/>
-      <c r="V38" s="63"/>
-      <c r="W38" s="64"/>
-      <c r="X38" s="65"/>
-      <c r="Y38" s="66"/>
-      <c r="Z38" s="66"/>
-      <c r="AA38" s="66"/>
-      <c r="AB38" s="10"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="55"/>
+      <c r="E38" s="55"/>
+      <c r="F38" s="55"/>
+      <c r="G38" s="55"/>
+      <c r="H38" s="55"/>
+      <c r="I38" s="44"/>
+      <c r="J38" s="44"/>
+      <c r="K38" s="44"/>
+      <c r="L38" s="44"/>
+      <c r="M38" s="44"/>
+      <c r="N38" s="44"/>
+      <c r="O38" s="44"/>
+      <c r="P38" s="44"/>
+      <c r="Q38" s="44"/>
+      <c r="R38" s="12"/>
+      <c r="S38" s="44"/>
+      <c r="T38" s="44"/>
+      <c r="U38" s="44"/>
+      <c r="V38" s="44"/>
+      <c r="W38" s="56"/>
+      <c r="X38" s="57"/>
+      <c r="Y38" s="55"/>
+      <c r="Z38" s="55"/>
+      <c r="AA38" s="55"/>
+      <c r="AB38" s="13"/>
     </row>
     <row r="39" spans="1:28" s="3" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="54" t="s">
+      <c r="A39" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="B39" s="55"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="55"/>
-      <c r="E39" s="55"/>
-      <c r="F39" s="56" t="s">
+      <c r="B39" s="50"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="G39" s="56"/>
-      <c r="H39" s="56"/>
-      <c r="I39" s="56"/>
-      <c r="J39" s="56"/>
-      <c r="K39" s="56"/>
-      <c r="L39" s="56"/>
-      <c r="M39" s="56"/>
-      <c r="N39" s="56"/>
-      <c r="O39" s="56"/>
-      <c r="P39" s="57" t="s">
+      <c r="G39" s="51"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="51"/>
+      <c r="L39" s="51"/>
+      <c r="M39" s="51"/>
+      <c r="N39" s="51"/>
+      <c r="O39" s="51"/>
+      <c r="P39" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="Q39" s="57"/>
-      <c r="R39" s="57"/>
-      <c r="S39" s="57"/>
-      <c r="T39" s="57"/>
-      <c r="U39" s="57" t="s">
+      <c r="Q39" s="52"/>
+      <c r="R39" s="52"/>
+      <c r="S39" s="52"/>
+      <c r="T39" s="52"/>
+      <c r="U39" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="V39" s="57"/>
-      <c r="W39" s="57"/>
-      <c r="X39" s="57"/>
-      <c r="Y39" s="57"/>
-      <c r="Z39" s="57" t="s">
+      <c r="V39" s="52"/>
+      <c r="W39" s="52"/>
+      <c r="X39" s="52"/>
+      <c r="Y39" s="52"/>
+      <c r="Z39" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="AA39" s="57"/>
-      <c r="AB39" s="58"/>
+      <c r="AA39" s="52"/>
+      <c r="AB39" s="53"/>
     </row>
     <row r="40" spans="1:28" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="49" t="s">
+      <c r="A40" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="50"/>
-      <c r="C40" s="50"/>
-      <c r="D40" s="50"/>
-      <c r="E40" s="50"/>
-      <c r="F40" s="52"/>
-      <c r="G40" s="52"/>
-      <c r="H40" s="52"/>
-      <c r="I40" s="52"/>
-      <c r="J40" s="52"/>
-      <c r="K40" s="52"/>
-      <c r="L40" s="52"/>
-      <c r="M40" s="52"/>
-      <c r="N40" s="52"/>
-      <c r="O40" s="52"/>
-      <c r="P40" s="59"/>
-      <c r="Q40" s="60"/>
-      <c r="R40" s="60"/>
-      <c r="S40" s="60"/>
-      <c r="T40" s="61"/>
-      <c r="U40" s="59"/>
-      <c r="V40" s="60"/>
-      <c r="W40" s="60"/>
-      <c r="X40" s="60"/>
-      <c r="Y40" s="61"/>
-      <c r="Z40" s="52"/>
-      <c r="AA40" s="52"/>
-      <c r="AB40" s="53"/>
+      <c r="B40" s="47"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="47"/>
+      <c r="E40" s="47"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="27"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="27"/>
+      <c r="N40" s="27"/>
+      <c r="O40" s="27"/>
+      <c r="P40" s="28"/>
+      <c r="Q40" s="54"/>
+      <c r="R40" s="54"/>
+      <c r="S40" s="54"/>
+      <c r="T40" s="29"/>
+      <c r="U40" s="28"/>
+      <c r="V40" s="54"/>
+      <c r="W40" s="54"/>
+      <c r="X40" s="54"/>
+      <c r="Y40" s="29"/>
+      <c r="Z40" s="27"/>
+      <c r="AA40" s="27"/>
+      <c r="AB40" s="48"/>
     </row>
     <row r="41" spans="1:28" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="49" t="s">
+      <c r="A41" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="B41" s="50"/>
-      <c r="C41" s="50"/>
-      <c r="D41" s="50"/>
-      <c r="E41" s="50"/>
-      <c r="F41" s="51"/>
-      <c r="G41" s="51"/>
-      <c r="H41" s="51"/>
-      <c r="I41" s="51"/>
-      <c r="J41" s="51"/>
-      <c r="K41" s="51"/>
-      <c r="L41" s="51"/>
-      <c r="M41" s="51"/>
-      <c r="N41" s="51"/>
-      <c r="O41" s="51"/>
-      <c r="P41" s="51"/>
-      <c r="Q41" s="51"/>
-      <c r="R41" s="51"/>
-      <c r="S41" s="51"/>
-      <c r="T41" s="51"/>
-      <c r="U41" s="52"/>
-      <c r="V41" s="52"/>
-      <c r="W41" s="52"/>
-      <c r="X41" s="52"/>
-      <c r="Y41" s="52"/>
-      <c r="Z41" s="52"/>
-      <c r="AA41" s="52"/>
-      <c r="AB41" s="53"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="47"/>
+      <c r="E41" s="47"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="27"/>
+      <c r="L41" s="27"/>
+      <c r="M41" s="27"/>
+      <c r="N41" s="27"/>
+      <c r="O41" s="27"/>
+      <c r="P41" s="27"/>
+      <c r="Q41" s="27"/>
+      <c r="R41" s="27"/>
+      <c r="S41" s="27"/>
+      <c r="T41" s="27"/>
+      <c r="U41" s="27"/>
+      <c r="V41" s="27"/>
+      <c r="W41" s="27"/>
+      <c r="X41" s="27"/>
+      <c r="Y41" s="27"/>
+      <c r="Z41" s="27"/>
+      <c r="AA41" s="27"/>
+      <c r="AB41" s="48"/>
     </row>
     <row r="42" spans="1:28" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="49" t="s">
+      <c r="A42" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B42" s="50"/>
-      <c r="C42" s="50"/>
-      <c r="D42" s="50"/>
-      <c r="E42" s="50"/>
-      <c r="F42" s="51"/>
-      <c r="G42" s="51"/>
-      <c r="H42" s="51"/>
-      <c r="I42" s="51"/>
-      <c r="J42" s="51"/>
-      <c r="K42" s="51"/>
-      <c r="L42" s="51"/>
-      <c r="M42" s="51"/>
-      <c r="N42" s="51"/>
-      <c r="O42" s="51"/>
-      <c r="P42" s="51"/>
-      <c r="Q42" s="51"/>
-      <c r="R42" s="51"/>
-      <c r="S42" s="51"/>
-      <c r="T42" s="51"/>
-      <c r="U42" s="52"/>
-      <c r="V42" s="52"/>
-      <c r="W42" s="52"/>
-      <c r="X42" s="52"/>
-      <c r="Y42" s="52"/>
-      <c r="Z42" s="52"/>
-      <c r="AA42" s="52"/>
-      <c r="AB42" s="53"/>
+      <c r="B42" s="47"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="47"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="27"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="27"/>
+      <c r="L42" s="27"/>
+      <c r="M42" s="27"/>
+      <c r="N42" s="27"/>
+      <c r="O42" s="27"/>
+      <c r="P42" s="27"/>
+      <c r="Q42" s="27"/>
+      <c r="R42" s="27"/>
+      <c r="S42" s="27"/>
+      <c r="T42" s="27"/>
+      <c r="U42" s="27"/>
+      <c r="V42" s="27"/>
+      <c r="W42" s="27"/>
+      <c r="X42" s="27"/>
+      <c r="Y42" s="27"/>
+      <c r="Z42" s="27"/>
+      <c r="AA42" s="27"/>
+      <c r="AB42" s="48"/>
     </row>
     <row r="43" spans="1:28" ht="57.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="45" t="s">
+      <c r="A43" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="B43" s="46"/>
-      <c r="C43" s="46"/>
-      <c r="D43" s="46"/>
-      <c r="E43" s="46"/>
-      <c r="F43" s="47"/>
-      <c r="G43" s="47"/>
-      <c r="H43" s="47"/>
-      <c r="I43" s="47"/>
-      <c r="J43" s="47"/>
-      <c r="K43" s="47"/>
-      <c r="L43" s="47"/>
-      <c r="M43" s="47"/>
-      <c r="N43" s="47"/>
-      <c r="O43" s="47"/>
-      <c r="P43" s="47"/>
-      <c r="Q43" s="47"/>
-      <c r="R43" s="47"/>
-      <c r="S43" s="47"/>
-      <c r="T43" s="47"/>
-      <c r="U43" s="47"/>
-      <c r="V43" s="47"/>
-      <c r="W43" s="47"/>
-      <c r="X43" s="47"/>
-      <c r="Y43" s="47"/>
-      <c r="Z43" s="47"/>
-      <c r="AA43" s="47"/>
-      <c r="AB43" s="48"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="44"/>
+      <c r="K43" s="44"/>
+      <c r="L43" s="44"/>
+      <c r="M43" s="44"/>
+      <c r="N43" s="44"/>
+      <c r="O43" s="44"/>
+      <c r="P43" s="44"/>
+      <c r="Q43" s="44"/>
+      <c r="R43" s="44"/>
+      <c r="S43" s="44"/>
+      <c r="T43" s="44"/>
+      <c r="U43" s="44"/>
+      <c r="V43" s="44"/>
+      <c r="W43" s="44"/>
+      <c r="X43" s="44"/>
+      <c r="Y43" s="44"/>
+      <c r="Z43" s="44"/>
+      <c r="AA43" s="44"/>
+      <c r="AB43" s="45"/>
     </row>
     <row r="44" spans="1:28" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="40" t="s">
+      <c r="A44" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="B44" s="41"/>
-      <c r="C44" s="41"/>
-      <c r="D44" s="41"/>
-      <c r="E44" s="41"/>
-      <c r="F44" s="41"/>
-      <c r="G44" s="41"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
-      <c r="K44" s="41"/>
-      <c r="L44" s="41"/>
-      <c r="M44" s="41"/>
-      <c r="N44" s="41"/>
-      <c r="O44" s="41"/>
-      <c r="P44" s="41"/>
-      <c r="Q44" s="41"/>
-      <c r="R44" s="41"/>
-      <c r="S44" s="41"/>
-      <c r="T44" s="41"/>
-      <c r="U44" s="41"/>
-      <c r="V44" s="41"/>
-      <c r="W44" s="41"/>
-      <c r="X44" s="41"/>
-      <c r="Y44" s="41"/>
-      <c r="Z44" s="41"/>
-      <c r="AA44" s="41"/>
-      <c r="AB44" s="41"/>
+      <c r="B44" s="39"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="39"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="39"/>
+      <c r="K44" s="39"/>
+      <c r="L44" s="39"/>
+      <c r="M44" s="39"/>
+      <c r="N44" s="39"/>
+      <c r="O44" s="39"/>
+      <c r="P44" s="39"/>
+      <c r="Q44" s="39"/>
+      <c r="R44" s="39"/>
+      <c r="S44" s="39"/>
+      <c r="T44" s="39"/>
+      <c r="U44" s="39"/>
+      <c r="V44" s="39"/>
+      <c r="W44" s="39"/>
+      <c r="X44" s="39"/>
+      <c r="Y44" s="39"/>
+      <c r="Z44" s="39"/>
+      <c r="AA44" s="39"/>
+      <c r="AB44" s="39"/>
     </row>
     <row r="45" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Replacing PDFbox with Aspose.cells
</commit_message>
<xml_diff>
--- a/src/assets/reports/report.xlsx
+++ b/src/assets/reports/report.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683BCD28-EAFC-4B75-8531-E950617802EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF0E92A-1BAA-422D-B73F-4FCD287D5644}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
   <si>
     <t>B</t>
   </si>
@@ -1116,10 +1116,28 @@
     </r>
   </si>
   <si>
-    <t>Doküman No: F.02 Yayın Tarihi : 01.05.2018 Revizyon No :01 Revizyon Tarihi :19.03.2019</t>
-  </si>
-  <si>
     <t xml:space="preserve"> GÖZETİM MUAYENE VE EĞİTİM HİZMETLERİ</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -1746,7 +1764,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1783,44 +1801,62 @@
     <xf numFmtId="49" fontId="20" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1828,10 +1864,7 @@
     <xf numFmtId="49" fontId="20" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1840,20 +1873,170 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1861,230 +2044,59 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -2124,20 +2136,28 @@
 </styleSheet>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$15" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$H$15" lockText="1" noThreeD="1"/>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
+      <xdr:colOff>24938</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:rowOff>108759</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>49877</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>198544</xdr:rowOff>
+      <xdr:rowOff>177763</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2167,8 +2187,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2209800" y="5417820"/>
-          <a:ext cx="1493520" cy="1074844"/>
+          <a:off x="2193174" y="5214159"/>
+          <a:ext cx="1472739" cy="1066531"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2248,132 +2268,140 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>152404</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>117759</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>277098</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>228598</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Rectangle 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C304B518-5F5B-4E51-8052-59AD0F31D9A4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1808022" y="6220686"/>
-          <a:ext cx="124694" cy="110839"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>457206</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>117762</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>581900</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>228601</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Rectangle 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C97102CD-1443-4A35-8050-47848BC7C78A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4128661" y="6220689"/>
-          <a:ext cx="124694" cy="110839"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>274320</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>83820</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>190500</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>53340</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Check Box 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>15</xdr:col>
+          <xdr:colOff>160020</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>91440</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>15</xdr:col>
+          <xdr:colOff>487680</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>53340</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="Check Box 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -2634,1527 +2662,1535 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AB429"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21:AB21"/>
+      <selection activeCell="U45" sqref="U45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.21875" style="1" customWidth="1"/>
-    <col min="2" max="3" width="5.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="0.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="4.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="0.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="4.21875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="3.21875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="3.44140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="5.77734375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="4.77734375" style="1" customWidth="1"/>
-    <col min="13" max="15" width="0.77734375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="8.77734375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="3.77734375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.77734375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="4.77734375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="3.77734375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="3.44140625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="0.77734375" style="1" customWidth="1"/>
-    <col min="23" max="23" width="10.77734375" style="1" customWidth="1"/>
-    <col min="24" max="24" width="2.44140625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="5.77734375" style="1" customWidth="1"/>
-    <col min="26" max="26" width="4.77734375" style="1" customWidth="1"/>
-    <col min="27" max="27" width="6.77734375" style="1" customWidth="1"/>
-    <col min="28" max="28" width="7.77734375" style="1" customWidth="1"/>
-    <col min="29" max="16384" width="8.77734375" style="1"/>
+    <col min="1" max="1" width="7.21875" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="5.21875" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="0.77734375" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="4.77734375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="0.77734375" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="4.21875" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="3.21875" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.5546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="3.44140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="5.77734375" style="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="4.77734375" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="15" width="0.77734375" style="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.77734375" style="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="3.77734375" style="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.77734375" style="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="4.77734375" style="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="3.77734375" style="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="3.44140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="0.77734375" style="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="10.77734375" style="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="2.44140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="5.77734375" style="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="4.77734375" style="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="6.77734375" style="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="7.77734375" style="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="16384" width="8.77734375" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="93"/>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="99" t="s">
-        <v>66</v>
-      </c>
-      <c r="I1" s="100"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="100"/>
-      <c r="L1" s="100"/>
-      <c r="M1" s="100"/>
-      <c r="N1" s="100"/>
-      <c r="O1" s="100"/>
-      <c r="P1" s="100"/>
-      <c r="Q1" s="100"/>
-      <c r="R1" s="100"/>
-      <c r="S1" s="100"/>
-      <c r="T1" s="100"/>
-      <c r="U1" s="100"/>
-      <c r="V1" s="100"/>
-      <c r="W1" s="100"/>
-      <c r="X1" s="100"/>
-      <c r="Y1" s="100"/>
-      <c r="Z1" s="100"/>
-      <c r="AA1" s="100"/>
-      <c r="AB1" s="101"/>
+      <c r="A1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="21"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
+      <c r="Y1" s="21"/>
+      <c r="Z1" s="21"/>
+      <c r="AA1" s="21"/>
+      <c r="AB1" s="22"/>
     </row>
     <row r="2" spans="1:28" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="96"/>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="102" t="s">
+      <c r="A2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
-      <c r="Q2" s="103"/>
-      <c r="R2" s="103"/>
-      <c r="S2" s="103"/>
-      <c r="T2" s="103"/>
-      <c r="U2" s="103"/>
-      <c r="V2" s="103"/>
-      <c r="W2" s="103"/>
-      <c r="X2" s="103"/>
-      <c r="Y2" s="103"/>
-      <c r="Z2" s="103"/>
-      <c r="AA2" s="103"/>
-      <c r="AB2" s="104"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="24"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="24"/>
+      <c r="Z2" s="24"/>
+      <c r="AA2" s="24"/>
+      <c r="AB2" s="25"/>
     </row>
     <row r="3" spans="1:28" s="3" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="106"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="107"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="107"/>
-      <c r="L3" s="107"/>
-      <c r="M3" s="107"/>
-      <c r="N3" s="107"/>
-      <c r="O3" s="107"/>
-      <c r="P3" s="107"/>
-      <c r="Q3" s="106" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="106"/>
-      <c r="S3" s="106"/>
-      <c r="T3" s="107"/>
-      <c r="U3" s="107"/>
-      <c r="V3" s="107"/>
-      <c r="W3" s="107"/>
-      <c r="X3" s="106" t="s">
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="28"/>
+      <c r="U3" s="28"/>
+      <c r="V3" s="28"/>
+      <c r="W3" s="28"/>
+      <c r="X3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="Y3" s="106"/>
-      <c r="Z3" s="106"/>
-      <c r="AA3" s="108"/>
-      <c r="AB3" s="109"/>
+      <c r="Y3" s="27"/>
+      <c r="Z3" s="27"/>
+      <c r="AA3" s="29"/>
+      <c r="AB3" s="30"/>
     </row>
     <row r="4" spans="1:28" s="3" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="36" t="s">
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="36"/>
-      <c r="S4" s="36"/>
-      <c r="T4" s="27"/>
-      <c r="U4" s="27"/>
-      <c r="V4" s="27"/>
-      <c r="W4" s="27"/>
-      <c r="X4" s="36" t="s">
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="33"/>
+      <c r="V4" s="33"/>
+      <c r="W4" s="33"/>
+      <c r="X4" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="Y4" s="36"/>
-      <c r="Z4" s="36"/>
-      <c r="AA4" s="28"/>
-      <c r="AB4" s="92"/>
+      <c r="Y4" s="32"/>
+      <c r="Z4" s="32"/>
+      <c r="AA4" s="34"/>
+      <c r="AB4" s="35"/>
     </row>
     <row r="5" spans="1:28" s="3" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="36" t="s">
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="R5" s="36"/>
-      <c r="S5" s="36"/>
-      <c r="T5" s="27"/>
-      <c r="U5" s="27"/>
-      <c r="V5" s="27"/>
-      <c r="W5" s="27"/>
-      <c r="X5" s="36" t="s">
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
+      <c r="T5" s="33"/>
+      <c r="U5" s="33"/>
+      <c r="V5" s="33"/>
+      <c r="W5" s="33"/>
+      <c r="X5" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="Y5" s="36"/>
-      <c r="Z5" s="36"/>
-      <c r="AA5" s="28"/>
-      <c r="AB5" s="92"/>
+      <c r="Y5" s="32"/>
+      <c r="Z5" s="32"/>
+      <c r="AA5" s="34"/>
+      <c r="AB5" s="35"/>
     </row>
     <row r="6" spans="1:28" s="3" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="54"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="36" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="42"/>
+      <c r="Q6" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="R6" s="36"/>
-      <c r="S6" s="36"/>
-      <c r="T6" s="27"/>
-      <c r="U6" s="27"/>
-      <c r="V6" s="27"/>
-      <c r="W6" s="27"/>
-      <c r="X6" s="36" t="s">
+      <c r="R6" s="32"/>
+      <c r="S6" s="32"/>
+      <c r="T6" s="33"/>
+      <c r="U6" s="33"/>
+      <c r="V6" s="33"/>
+      <c r="W6" s="33"/>
+      <c r="X6" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="Y6" s="36"/>
-      <c r="Z6" s="36"/>
-      <c r="AA6" s="28"/>
-      <c r="AB6" s="92"/>
+      <c r="Y6" s="32"/>
+      <c r="Z6" s="32"/>
+      <c r="AA6" s="34"/>
+      <c r="AB6" s="35"/>
     </row>
     <row r="7" spans="1:28" s="3" customFormat="1" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="44"/>
-      <c r="M7" s="44"/>
-      <c r="N7" s="44"/>
-      <c r="O7" s="44"/>
-      <c r="P7" s="44"/>
-      <c r="Q7" s="32" t="s">
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="R7" s="32"/>
-      <c r="S7" s="32"/>
-      <c r="T7" s="44"/>
-      <c r="U7" s="44"/>
-      <c r="V7" s="44"/>
-      <c r="W7" s="44"/>
-      <c r="X7" s="32" t="s">
+      <c r="R7" s="37"/>
+      <c r="S7" s="37"/>
+      <c r="T7" s="38"/>
+      <c r="U7" s="38"/>
+      <c r="V7" s="38"/>
+      <c r="W7" s="38"/>
+      <c r="X7" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="Y7" s="32"/>
-      <c r="Z7" s="32"/>
-      <c r="AA7" s="56"/>
-      <c r="AB7" s="91"/>
+      <c r="Y7" s="37"/>
+      <c r="Z7" s="37"/>
+      <c r="AA7" s="39"/>
+      <c r="AB7" s="40"/>
     </row>
     <row r="8" spans="1:28" s="3" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="88" t="s">
+      <c r="A8" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="89"/>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
-      <c r="G8" s="89"/>
-      <c r="H8" s="89"/>
-      <c r="I8" s="89"/>
-      <c r="J8" s="89"/>
-      <c r="K8" s="89"/>
-      <c r="L8" s="89"/>
-      <c r="M8" s="89"/>
-      <c r="N8" s="89"/>
-      <c r="O8" s="89"/>
-      <c r="P8" s="89"/>
-      <c r="Q8" s="89"/>
-      <c r="R8" s="89"/>
-      <c r="S8" s="89"/>
-      <c r="T8" s="89"/>
-      <c r="U8" s="89"/>
-      <c r="V8" s="89"/>
-      <c r="W8" s="89"/>
-      <c r="X8" s="89"/>
-      <c r="Y8" s="89"/>
-      <c r="Z8" s="89"/>
-      <c r="AA8" s="89"/>
-      <c r="AB8" s="90"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="45"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="45"/>
+      <c r="P8" s="45"/>
+      <c r="Q8" s="45"/>
+      <c r="R8" s="45"/>
+      <c r="S8" s="45"/>
+      <c r="T8" s="45"/>
+      <c r="U8" s="45"/>
+      <c r="V8" s="45"/>
+      <c r="W8" s="45"/>
+      <c r="X8" s="45"/>
+      <c r="Y8" s="45"/>
+      <c r="Z8" s="45"/>
+      <c r="AA8" s="45"/>
+      <c r="AB8" s="46"/>
     </row>
     <row r="9" spans="1:28" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="36" t="s">
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="36"/>
-      <c r="Q9" s="37"/>
-      <c r="R9" s="37"/>
-      <c r="S9" s="37"/>
-      <c r="T9" s="37"/>
-      <c r="U9" s="37"/>
-      <c r="V9" s="37"/>
-      <c r="W9" s="36" t="s">
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="43"/>
+      <c r="R9" s="43"/>
+      <c r="S9" s="43"/>
+      <c r="T9" s="43"/>
+      <c r="U9" s="43"/>
+      <c r="V9" s="43"/>
+      <c r="W9" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="X9" s="36"/>
-      <c r="Y9" s="36"/>
-      <c r="Z9" s="37"/>
-      <c r="AA9" s="37"/>
-      <c r="AB9" s="41"/>
+      <c r="X9" s="32"/>
+      <c r="Y9" s="32"/>
+      <c r="Z9" s="43"/>
+      <c r="AA9" s="43"/>
+      <c r="AB9" s="47"/>
     </row>
     <row r="10" spans="1:28" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="36" t="s">
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
-      <c r="N10" s="36"/>
-      <c r="O10" s="36"/>
-      <c r="P10" s="36"/>
-      <c r="Q10" s="37"/>
-      <c r="R10" s="37"/>
-      <c r="S10" s="37"/>
-      <c r="T10" s="37"/>
-      <c r="U10" s="37"/>
-      <c r="V10" s="37"/>
-      <c r="W10" s="40" t="s">
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="43"/>
+      <c r="S10" s="43"/>
+      <c r="T10" s="43"/>
+      <c r="U10" s="43"/>
+      <c r="V10" s="43"/>
+      <c r="W10" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="X10" s="40"/>
-      <c r="Y10" s="40"/>
-      <c r="Z10" s="37"/>
-      <c r="AA10" s="37"/>
-      <c r="AB10" s="41"/>
+      <c r="X10" s="69"/>
+      <c r="Y10" s="69"/>
+      <c r="Z10" s="43"/>
+      <c r="AA10" s="43"/>
+      <c r="AB10" s="47"/>
     </row>
     <row r="11" spans="1:28" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="36" t="s">
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="36"/>
-      <c r="M11" s="36"/>
-      <c r="N11" s="36"/>
-      <c r="O11" s="36"/>
-      <c r="P11" s="36"/>
-      <c r="Q11" s="37"/>
-      <c r="R11" s="37"/>
-      <c r="S11" s="37"/>
-      <c r="T11" s="37"/>
-      <c r="U11" s="37"/>
-      <c r="V11" s="37"/>
-      <c r="W11" s="40"/>
-      <c r="X11" s="40"/>
-      <c r="Y11" s="40"/>
-      <c r="Z11" s="37"/>
-      <c r="AA11" s="37"/>
-      <c r="AB11" s="41"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="43"/>
+      <c r="S11" s="43"/>
+      <c r="T11" s="43"/>
+      <c r="U11" s="43"/>
+      <c r="V11" s="43"/>
+      <c r="W11" s="69"/>
+      <c r="X11" s="69"/>
+      <c r="Y11" s="69"/>
+      <c r="Z11" s="43"/>
+      <c r="AA11" s="43"/>
+      <c r="AB11" s="47"/>
     </row>
     <row r="12" spans="1:28" s="4" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="36" t="s">
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="36"/>
-      <c r="P12" s="36"/>
-      <c r="Q12" s="37"/>
-      <c r="R12" s="37"/>
-      <c r="S12" s="37"/>
-      <c r="T12" s="37"/>
-      <c r="U12" s="37"/>
-      <c r="V12" s="37"/>
-      <c r="W12" s="36" t="s">
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="43"/>
+      <c r="S12" s="43"/>
+      <c r="T12" s="43"/>
+      <c r="U12" s="43"/>
+      <c r="V12" s="43"/>
+      <c r="W12" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="X12" s="36"/>
-      <c r="Y12" s="36"/>
-      <c r="Z12" s="26"/>
-      <c r="AA12" s="26"/>
-      <c r="AB12" s="30"/>
+      <c r="X12" s="32"/>
+      <c r="Y12" s="32"/>
+      <c r="Z12" s="85"/>
+      <c r="AA12" s="85"/>
+      <c r="AB12" s="98"/>
     </row>
     <row r="13" spans="1:28" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="36" t="s">
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="36"/>
-      <c r="O13" s="36"/>
-      <c r="P13" s="36"/>
-      <c r="Q13" s="37"/>
-      <c r="R13" s="37"/>
-      <c r="S13" s="37"/>
-      <c r="T13" s="37"/>
-      <c r="U13" s="37"/>
-      <c r="V13" s="37"/>
-      <c r="W13" s="14" t="s">
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="R13" s="43"/>
+      <c r="S13" s="43"/>
+      <c r="T13" s="43"/>
+      <c r="U13" s="43"/>
+      <c r="V13" s="43"/>
+      <c r="W13" s="101" t="s">
         <v>63</v>
       </c>
-      <c r="X13" s="15"/>
-      <c r="Y13" s="16"/>
-      <c r="Z13" s="20"/>
-      <c r="AA13" s="21"/>
-      <c r="AB13" s="22"/>
+      <c r="X13" s="102"/>
+      <c r="Y13" s="103"/>
+      <c r="Z13" s="107"/>
+      <c r="AA13" s="108"/>
+      <c r="AB13" s="109"/>
     </row>
     <row r="14" spans="1:28" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="32" t="s">
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="99"/>
+      <c r="F14" s="99"/>
+      <c r="G14" s="99"/>
+      <c r="H14" s="99"/>
+      <c r="I14" s="99"/>
+      <c r="J14" s="99"/>
+      <c r="K14" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="32"/>
-      <c r="O14" s="32"/>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="34"/>
-      <c r="R14" s="34"/>
-      <c r="S14" s="34"/>
-      <c r="T14" s="34"/>
-      <c r="U14" s="34"/>
-      <c r="V14" s="34"/>
-      <c r="W14" s="17" t="s">
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="100" t="s">
+        <v>72</v>
+      </c>
+      <c r="R14" s="100"/>
+      <c r="S14" s="100"/>
+      <c r="T14" s="100"/>
+      <c r="U14" s="100"/>
+      <c r="V14" s="100"/>
+      <c r="W14" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="19"/>
-      <c r="Z14" s="23"/>
-      <c r="AA14" s="24"/>
-      <c r="AB14" s="25"/>
+      <c r="X14" s="105"/>
+      <c r="Y14" s="106"/>
+      <c r="Z14" s="110"/>
+      <c r="AA14" s="111"/>
+      <c r="AB14" s="112"/>
     </row>
     <row r="15" spans="1:28" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="75"/>
-      <c r="B15" s="76"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="76"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="76"/>
-      <c r="H15" s="79"/>
-      <c r="I15" s="79"/>
-      <c r="J15" s="79"/>
-      <c r="K15" s="79"/>
-      <c r="L15" s="79"/>
-      <c r="M15" s="79"/>
-      <c r="N15" s="79"/>
-      <c r="O15" s="79"/>
-      <c r="P15" s="80"/>
-      <c r="Q15" s="85" t="s">
+      <c r="A15" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="B15" s="55"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="55"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="55"/>
+      <c r="M15" s="55"/>
+      <c r="N15" s="55"/>
+      <c r="O15" s="55"/>
+      <c r="P15" s="58"/>
+      <c r="Q15" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="R15" s="86"/>
-      <c r="S15" s="86"/>
-      <c r="T15" s="86"/>
-      <c r="U15" s="86"/>
-      <c r="V15" s="86"/>
-      <c r="W15" s="86"/>
-      <c r="X15" s="86"/>
-      <c r="Y15" s="86"/>
-      <c r="Z15" s="86"/>
-      <c r="AA15" s="86"/>
-      <c r="AB15" s="87"/>
+      <c r="R15" s="63"/>
+      <c r="S15" s="63"/>
+      <c r="T15" s="63"/>
+      <c r="U15" s="63"/>
+      <c r="V15" s="63"/>
+      <c r="W15" s="63"/>
+      <c r="X15" s="63"/>
+      <c r="Y15" s="63"/>
+      <c r="Z15" s="63"/>
+      <c r="AA15" s="63"/>
+      <c r="AB15" s="64"/>
     </row>
     <row r="16" spans="1:28" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="77"/>
-      <c r="B16" s="78"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="78"/>
-      <c r="H16" s="81"/>
-      <c r="I16" s="81"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="81"/>
-      <c r="L16" s="81"/>
-      <c r="M16" s="81"/>
-      <c r="N16" s="81"/>
-      <c r="O16" s="81"/>
-      <c r="P16" s="82"/>
-      <c r="Q16" s="83" t="s">
+      <c r="A16" s="56"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="57"/>
+      <c r="K16" s="57"/>
+      <c r="L16" s="57"/>
+      <c r="M16" s="57"/>
+      <c r="N16" s="57"/>
+      <c r="O16" s="57"/>
+      <c r="P16" s="59"/>
+      <c r="Q16" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="R16" s="84"/>
-      <c r="S16" s="69" t="s">
+      <c r="R16" s="61"/>
+      <c r="S16" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="T16" s="69"/>
-      <c r="U16" s="69"/>
-      <c r="V16" s="69"/>
-      <c r="W16" s="69"/>
-      <c r="X16" s="69"/>
-      <c r="Y16" s="69"/>
-      <c r="Z16" s="69"/>
-      <c r="AA16" s="69"/>
-      <c r="AB16" s="70"/>
+      <c r="T16" s="48"/>
+      <c r="U16" s="48"/>
+      <c r="V16" s="48"/>
+      <c r="W16" s="48"/>
+      <c r="X16" s="48"/>
+      <c r="Y16" s="48"/>
+      <c r="Z16" s="48"/>
+      <c r="AA16" s="48"/>
+      <c r="AB16" s="49"/>
     </row>
     <row r="17" spans="1:28" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="77"/>
-      <c r="B17" s="78"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="81"/>
-      <c r="I17" s="81"/>
-      <c r="J17" s="81"/>
-      <c r="K17" s="81"/>
-      <c r="L17" s="81"/>
-      <c r="M17" s="81"/>
-      <c r="N17" s="81"/>
-      <c r="O17" s="81"/>
-      <c r="P17" s="82"/>
-      <c r="Q17" s="83" t="s">
+      <c r="A17" s="56"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="57"/>
+      <c r="K17" s="57"/>
+      <c r="L17" s="57"/>
+      <c r="M17" s="57"/>
+      <c r="N17" s="57"/>
+      <c r="O17" s="57"/>
+      <c r="P17" s="59"/>
+      <c r="Q17" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="R17" s="84"/>
-      <c r="S17" s="69" t="s">
+      <c r="R17" s="61"/>
+      <c r="S17" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="T17" s="69"/>
-      <c r="U17" s="69"/>
-      <c r="V17" s="69"/>
-      <c r="W17" s="69"/>
-      <c r="X17" s="69"/>
-      <c r="Y17" s="69"/>
-      <c r="Z17" s="69"/>
-      <c r="AA17" s="69"/>
-      <c r="AB17" s="70"/>
+      <c r="T17" s="48"/>
+      <c r="U17" s="48"/>
+      <c r="V17" s="48"/>
+      <c r="W17" s="48"/>
+      <c r="X17" s="48"/>
+      <c r="Y17" s="48"/>
+      <c r="Z17" s="48"/>
+      <c r="AA17" s="48"/>
+      <c r="AB17" s="49"/>
     </row>
     <row r="18" spans="1:28" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="77"/>
-      <c r="B18" s="78"/>
-      <c r="C18" s="78"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="78"/>
-      <c r="F18" s="78"/>
-      <c r="G18" s="78"/>
-      <c r="H18" s="81"/>
-      <c r="I18" s="81"/>
-      <c r="J18" s="81"/>
-      <c r="K18" s="81"/>
-      <c r="L18" s="81"/>
-      <c r="M18" s="81"/>
-      <c r="N18" s="81"/>
-      <c r="O18" s="81"/>
-      <c r="P18" s="82"/>
-      <c r="Q18" s="83" t="s">
+      <c r="A18" s="56"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="57"/>
+      <c r="O18" s="57"/>
+      <c r="P18" s="59"/>
+      <c r="Q18" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="R18" s="84"/>
-      <c r="S18" s="69" t="s">
+      <c r="R18" s="61"/>
+      <c r="S18" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="T18" s="69"/>
-      <c r="U18" s="69"/>
-      <c r="V18" s="69"/>
-      <c r="W18" s="69"/>
-      <c r="X18" s="69"/>
-      <c r="Y18" s="69"/>
-      <c r="Z18" s="69"/>
-      <c r="AA18" s="69"/>
-      <c r="AB18" s="70"/>
+      <c r="T18" s="48"/>
+      <c r="U18" s="48"/>
+      <c r="V18" s="48"/>
+      <c r="W18" s="48"/>
+      <c r="X18" s="48"/>
+      <c r="Y18" s="48"/>
+      <c r="Z18" s="48"/>
+      <c r="AA18" s="48"/>
+      <c r="AB18" s="49"/>
     </row>
     <row r="19" spans="1:28" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="77"/>
-      <c r="B19" s="78"/>
-      <c r="C19" s="78"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="78"/>
-      <c r="H19" s="81"/>
-      <c r="I19" s="81"/>
-      <c r="J19" s="81"/>
-      <c r="K19" s="81"/>
-      <c r="L19" s="81"/>
-      <c r="M19" s="81"/>
-      <c r="N19" s="81"/>
-      <c r="O19" s="81"/>
-      <c r="P19" s="82"/>
-      <c r="Q19" s="71" t="s">
+      <c r="A19" s="56"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="57"/>
+      <c r="L19" s="57"/>
+      <c r="M19" s="57"/>
+      <c r="N19" s="57"/>
+      <c r="O19" s="57"/>
+      <c r="P19" s="59"/>
+      <c r="Q19" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="R19" s="72"/>
-      <c r="S19" s="73" t="s">
+      <c r="R19" s="51"/>
+      <c r="S19" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="T19" s="73"/>
-      <c r="U19" s="73"/>
-      <c r="V19" s="73"/>
-      <c r="W19" s="73"/>
-      <c r="X19" s="73"/>
-      <c r="Y19" s="73"/>
-      <c r="Z19" s="73"/>
-      <c r="AA19" s="73"/>
-      <c r="AB19" s="74"/>
+      <c r="T19" s="52"/>
+      <c r="U19" s="52"/>
+      <c r="V19" s="52"/>
+      <c r="W19" s="52"/>
+      <c r="X19" s="52"/>
+      <c r="Y19" s="52"/>
+      <c r="Z19" s="52"/>
+      <c r="AA19" s="52"/>
+      <c r="AB19" s="53"/>
     </row>
     <row r="20" spans="1:28" ht="26.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="62" t="s">
+      <c r="A20" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="63"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
-      <c r="G20" s="63"/>
-      <c r="H20" s="110"/>
-      <c r="I20" s="110"/>
-      <c r="J20" s="110"/>
-      <c r="K20" s="110"/>
-      <c r="L20" s="110"/>
-      <c r="M20" s="110"/>
-      <c r="N20" s="110"/>
-      <c r="O20" s="110"/>
-      <c r="P20" s="110"/>
-      <c r="Q20" s="111"/>
-      <c r="R20" s="111"/>
-      <c r="S20" s="111"/>
-      <c r="T20" s="111"/>
-      <c r="U20" s="111"/>
-      <c r="V20" s="111"/>
-      <c r="W20" s="111"/>
-      <c r="X20" s="111"/>
-      <c r="Y20" s="111"/>
-      <c r="Z20" s="111"/>
-      <c r="AA20" s="111"/>
-      <c r="AB20" s="112"/>
+      <c r="B20" s="73"/>
+      <c r="C20" s="73"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="73"/>
+      <c r="H20" s="74"/>
+      <c r="I20" s="74"/>
+      <c r="J20" s="74"/>
+      <c r="K20" s="74"/>
+      <c r="L20" s="74"/>
+      <c r="M20" s="74"/>
+      <c r="N20" s="74"/>
+      <c r="O20" s="74"/>
+      <c r="P20" s="74"/>
+      <c r="Q20" s="75"/>
+      <c r="R20" s="75"/>
+      <c r="S20" s="75"/>
+      <c r="T20" s="75"/>
+      <c r="U20" s="75"/>
+      <c r="V20" s="75"/>
+      <c r="W20" s="75"/>
+      <c r="X20" s="75"/>
+      <c r="Y20" s="75"/>
+      <c r="Z20" s="75"/>
+      <c r="AA20" s="75"/>
+      <c r="AB20" s="76"/>
     </row>
     <row r="21" spans="1:28" ht="26.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="64" t="s">
+      <c r="A21" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="65"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="113"/>
-      <c r="I21" s="113"/>
-      <c r="J21" s="113"/>
-      <c r="K21" s="113"/>
-      <c r="L21" s="113"/>
-      <c r="M21" s="113"/>
-      <c r="N21" s="113"/>
-      <c r="O21" s="113"/>
-      <c r="P21" s="113"/>
-      <c r="Q21" s="113"/>
-      <c r="R21" s="113"/>
-      <c r="S21" s="113"/>
-      <c r="T21" s="113"/>
-      <c r="U21" s="113"/>
-      <c r="V21" s="113"/>
-      <c r="W21" s="113"/>
-      <c r="X21" s="113"/>
-      <c r="Y21" s="113"/>
-      <c r="Z21" s="113"/>
-      <c r="AA21" s="113"/>
-      <c r="AB21" s="114"/>
+      <c r="B21" s="78"/>
+      <c r="C21" s="78"/>
+      <c r="D21" s="78"/>
+      <c r="E21" s="78"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="78"/>
+      <c r="H21" s="79"/>
+      <c r="I21" s="79"/>
+      <c r="J21" s="79"/>
+      <c r="K21" s="79"/>
+      <c r="L21" s="79"/>
+      <c r="M21" s="79"/>
+      <c r="N21" s="79"/>
+      <c r="O21" s="79"/>
+      <c r="P21" s="79"/>
+      <c r="Q21" s="79"/>
+      <c r="R21" s="79"/>
+      <c r="S21" s="79"/>
+      <c r="T21" s="79"/>
+      <c r="U21" s="79"/>
+      <c r="V21" s="79"/>
+      <c r="W21" s="79"/>
+      <c r="X21" s="79"/>
+      <c r="Y21" s="79"/>
+      <c r="Z21" s="79"/>
+      <c r="AA21" s="79"/>
+      <c r="AB21" s="80"/>
     </row>
     <row r="22" spans="1:28" ht="26.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="67"/>
-      <c r="C22" s="67"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="67"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="55"/>
-      <c r="J22" s="55"/>
-      <c r="K22" s="55"/>
-      <c r="L22" s="55"/>
-      <c r="M22" s="55"/>
-      <c r="N22" s="55"/>
-      <c r="O22" s="55"/>
-      <c r="P22" s="55"/>
-      <c r="Q22" s="55"/>
-      <c r="R22" s="55"/>
-      <c r="S22" s="55"/>
-      <c r="T22" s="55"/>
-      <c r="U22" s="55"/>
-      <c r="V22" s="55"/>
-      <c r="W22" s="55"/>
-      <c r="X22" s="55"/>
-      <c r="Y22" s="55"/>
-      <c r="Z22" s="55"/>
-      <c r="AA22" s="55"/>
-      <c r="AB22" s="68"/>
+      <c r="B22" s="82"/>
+      <c r="C22" s="82"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="82"/>
+      <c r="G22" s="82"/>
+      <c r="H22" s="83" t="s">
+        <v>72</v>
+      </c>
+      <c r="I22" s="83"/>
+      <c r="J22" s="83"/>
+      <c r="K22" s="83"/>
+      <c r="L22" s="83"/>
+      <c r="M22" s="83"/>
+      <c r="N22" s="83"/>
+      <c r="O22" s="83"/>
+      <c r="P22" s="83"/>
+      <c r="Q22" s="83"/>
+      <c r="R22" s="83"/>
+      <c r="S22" s="83"/>
+      <c r="T22" s="83"/>
+      <c r="U22" s="83"/>
+      <c r="V22" s="83"/>
+      <c r="W22" s="83"/>
+      <c r="X22" s="83"/>
+      <c r="Y22" s="83"/>
+      <c r="Z22" s="83"/>
+      <c r="AA22" s="83"/>
+      <c r="AB22" s="84"/>
     </row>
     <row r="23" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="58" t="s">
+      <c r="A23" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="52"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="52"/>
-      <c r="L23" s="52"/>
-      <c r="M23" s="52"/>
-      <c r="N23" s="52"/>
-      <c r="O23" s="52"/>
-      <c r="P23" s="52"/>
-      <c r="Q23" s="52"/>
-      <c r="R23" s="52"/>
-      <c r="S23" s="52"/>
-      <c r="T23" s="52"/>
-      <c r="U23" s="52"/>
-      <c r="V23" s="52"/>
-      <c r="W23" s="52"/>
-      <c r="X23" s="52"/>
-      <c r="Y23" s="52"/>
-      <c r="Z23" s="52"/>
-      <c r="AA23" s="52"/>
-      <c r="AB23" s="53"/>
+      <c r="B23" s="66"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="66"/>
+      <c r="J23" s="66"/>
+      <c r="K23" s="66"/>
+      <c r="L23" s="66"/>
+      <c r="M23" s="66"/>
+      <c r="N23" s="66"/>
+      <c r="O23" s="66"/>
+      <c r="P23" s="66"/>
+      <c r="Q23" s="66"/>
+      <c r="R23" s="66"/>
+      <c r="S23" s="66"/>
+      <c r="T23" s="66"/>
+      <c r="U23" s="66"/>
+      <c r="V23" s="66"/>
+      <c r="W23" s="66"/>
+      <c r="X23" s="66"/>
+      <c r="Y23" s="66"/>
+      <c r="Z23" s="66"/>
+      <c r="AA23" s="66"/>
+      <c r="AB23" s="67"/>
     </row>
     <row r="24" spans="1:28" s="3" customFormat="1" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="59" t="s">
+      <c r="B24" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="59"/>
-      <c r="I24" s="59" t="s">
+      <c r="C24" s="68"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="J24" s="59"/>
-      <c r="K24" s="59"/>
-      <c r="L24" s="40" t="s">
+      <c r="J24" s="68"/>
+      <c r="K24" s="68"/>
+      <c r="L24" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="M24" s="40"/>
-      <c r="N24" s="40"/>
-      <c r="O24" s="40"/>
-      <c r="P24" s="40"/>
-      <c r="Q24" s="40"/>
+      <c r="M24" s="69"/>
+      <c r="N24" s="69"/>
+      <c r="O24" s="69"/>
+      <c r="P24" s="69"/>
+      <c r="Q24" s="69"/>
       <c r="R24" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="S24" s="59" t="s">
+      <c r="S24" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="T24" s="59"/>
-      <c r="U24" s="59"/>
-      <c r="V24" s="59"/>
-      <c r="W24" s="60" t="s">
+      <c r="T24" s="68"/>
+      <c r="U24" s="68"/>
+      <c r="V24" s="68"/>
+      <c r="W24" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="X24" s="61"/>
-      <c r="Y24" s="59" t="s">
+      <c r="X24" s="71"/>
+      <c r="Y24" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="Z24" s="59"/>
-      <c r="AA24" s="59"/>
+      <c r="Z24" s="68"/>
+      <c r="AA24" s="68"/>
       <c r="AB24" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
-        <v>1</v>
-      </c>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="27"/>
-      <c r="N25" s="27"/>
-      <c r="O25" s="27"/>
-      <c r="P25" s="27"/>
-      <c r="Q25" s="27"/>
+      <c r="A25" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="85"/>
+      <c r="C25" s="85"/>
+      <c r="D25" s="85"/>
+      <c r="E25" s="85"/>
+      <c r="F25" s="85"/>
+      <c r="G25" s="85"/>
+      <c r="H25" s="85"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="33"/>
+      <c r="P25" s="33"/>
+      <c r="Q25" s="33"/>
       <c r="R25" s="8"/>
-      <c r="S25" s="27"/>
-      <c r="T25" s="27"/>
-      <c r="U25" s="27"/>
-      <c r="V25" s="27"/>
-      <c r="W25" s="28"/>
-      <c r="X25" s="29"/>
-      <c r="Y25" s="26"/>
-      <c r="Z25" s="26"/>
-      <c r="AA25" s="26"/>
+      <c r="S25" s="33"/>
+      <c r="T25" s="33"/>
+      <c r="U25" s="33"/>
+      <c r="V25" s="33"/>
+      <c r="W25" s="34"/>
+      <c r="X25" s="42"/>
+      <c r="Y25" s="85"/>
+      <c r="Z25" s="85"/>
+      <c r="AA25" s="85"/>
       <c r="AB25" s="10"/>
     </row>
     <row r="26" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
-        <v>2</v>
-      </c>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="27"/>
-      <c r="M26" s="27"/>
-      <c r="N26" s="27"/>
-      <c r="O26" s="27"/>
-      <c r="P26" s="27"/>
-      <c r="Q26" s="27"/>
+      <c r="A26" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="85"/>
+      <c r="C26" s="85"/>
+      <c r="D26" s="85"/>
+      <c r="E26" s="85"/>
+      <c r="F26" s="85"/>
+      <c r="G26" s="85"/>
+      <c r="H26" s="85"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="33"/>
+      <c r="N26" s="33"/>
+      <c r="O26" s="33"/>
+      <c r="P26" s="33"/>
+      <c r="Q26" s="33"/>
       <c r="R26" s="8"/>
-      <c r="S26" s="27"/>
-      <c r="T26" s="27"/>
-      <c r="U26" s="27"/>
-      <c r="V26" s="27"/>
-      <c r="W26" s="28"/>
-      <c r="X26" s="29"/>
-      <c r="Y26" s="26"/>
-      <c r="Z26" s="26"/>
-      <c r="AA26" s="26"/>
+      <c r="S26" s="33"/>
+      <c r="T26" s="33"/>
+      <c r="U26" s="33"/>
+      <c r="V26" s="33"/>
+      <c r="W26" s="34"/>
+      <c r="X26" s="42"/>
+      <c r="Y26" s="85"/>
+      <c r="Z26" s="85"/>
+      <c r="AA26" s="85"/>
       <c r="AB26" s="10"/>
     </row>
     <row r="27" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
-        <v>3</v>
-      </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="27"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="27"/>
-      <c r="N27" s="27"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="27"/>
-      <c r="Q27" s="27"/>
+      <c r="A27" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="85"/>
+      <c r="C27" s="85"/>
+      <c r="D27" s="85"/>
+      <c r="E27" s="85"/>
+      <c r="F27" s="85"/>
+      <c r="G27" s="85"/>
+      <c r="H27" s="85"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="33"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="33"/>
+      <c r="O27" s="33"/>
+      <c r="P27" s="33"/>
+      <c r="Q27" s="33"/>
       <c r="R27" s="8"/>
-      <c r="S27" s="27"/>
-      <c r="T27" s="27"/>
-      <c r="U27" s="27"/>
-      <c r="V27" s="27"/>
-      <c r="W27" s="28"/>
-      <c r="X27" s="29"/>
-      <c r="Y27" s="26"/>
-      <c r="Z27" s="26"/>
-      <c r="AA27" s="26"/>
+      <c r="S27" s="33"/>
+      <c r="T27" s="33"/>
+      <c r="U27" s="33"/>
+      <c r="V27" s="33"/>
+      <c r="W27" s="34"/>
+      <c r="X27" s="42"/>
+      <c r="Y27" s="85"/>
+      <c r="Z27" s="85"/>
+      <c r="AA27" s="85"/>
       <c r="AB27" s="10"/>
     </row>
     <row r="28" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
-        <v>4</v>
-      </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="27"/>
-      <c r="K28" s="27"/>
-      <c r="L28" s="27"/>
-      <c r="M28" s="27"/>
-      <c r="N28" s="27"/>
-      <c r="O28" s="27"/>
-      <c r="P28" s="27"/>
-      <c r="Q28" s="27"/>
+      <c r="A28" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="85"/>
+      <c r="C28" s="85"/>
+      <c r="D28" s="85"/>
+      <c r="E28" s="85"/>
+      <c r="F28" s="85"/>
+      <c r="G28" s="85"/>
+      <c r="H28" s="85"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="33"/>
+      <c r="O28" s="33"/>
+      <c r="P28" s="33"/>
+      <c r="Q28" s="33"/>
       <c r="R28" s="8"/>
-      <c r="S28" s="27"/>
-      <c r="T28" s="27"/>
-      <c r="U28" s="27"/>
-      <c r="V28" s="27"/>
-      <c r="W28" s="28"/>
-      <c r="X28" s="29"/>
-      <c r="Y28" s="26"/>
-      <c r="Z28" s="26"/>
-      <c r="AA28" s="26"/>
+      <c r="S28" s="33"/>
+      <c r="T28" s="33"/>
+      <c r="U28" s="33"/>
+      <c r="V28" s="33"/>
+      <c r="W28" s="34"/>
+      <c r="X28" s="42"/>
+      <c r="Y28" s="85"/>
+      <c r="Z28" s="85"/>
+      <c r="AA28" s="85"/>
       <c r="AB28" s="10"/>
     </row>
     <row r="29" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
-        <v>5</v>
-      </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="27"/>
-      <c r="Q29" s="27"/>
+      <c r="A29" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="85"/>
+      <c r="C29" s="85"/>
+      <c r="D29" s="85"/>
+      <c r="E29" s="85"/>
+      <c r="F29" s="85"/>
+      <c r="G29" s="85"/>
+      <c r="H29" s="85"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="33"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="33"/>
+      <c r="O29" s="33"/>
+      <c r="P29" s="33"/>
+      <c r="Q29" s="33"/>
       <c r="R29" s="8"/>
-      <c r="S29" s="27"/>
-      <c r="T29" s="27"/>
-      <c r="U29" s="27"/>
-      <c r="V29" s="27"/>
-      <c r="W29" s="28"/>
-      <c r="X29" s="29"/>
-      <c r="Y29" s="26"/>
-      <c r="Z29" s="26"/>
-      <c r="AA29" s="26"/>
+      <c r="S29" s="33"/>
+      <c r="T29" s="33"/>
+      <c r="U29" s="33"/>
+      <c r="V29" s="33"/>
+      <c r="W29" s="34"/>
+      <c r="X29" s="42"/>
+      <c r="Y29" s="85"/>
+      <c r="Z29" s="85"/>
+      <c r="AA29" s="85"/>
       <c r="AB29" s="10"/>
     </row>
     <row r="30" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
-        <v>6</v>
-      </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
-      <c r="K30" s="27"/>
-      <c r="L30" s="27"/>
-      <c r="M30" s="27"/>
-      <c r="N30" s="27"/>
-      <c r="O30" s="27"/>
-      <c r="P30" s="27"/>
-      <c r="Q30" s="27"/>
+      <c r="A30" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="85"/>
+      <c r="C30" s="85"/>
+      <c r="D30" s="85"/>
+      <c r="E30" s="85"/>
+      <c r="F30" s="85"/>
+      <c r="G30" s="85"/>
+      <c r="H30" s="85"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="33"/>
+      <c r="O30" s="33"/>
+      <c r="P30" s="33"/>
+      <c r="Q30" s="33"/>
       <c r="R30" s="8"/>
-      <c r="S30" s="27"/>
-      <c r="T30" s="27"/>
-      <c r="U30" s="27"/>
-      <c r="V30" s="27"/>
-      <c r="W30" s="28"/>
-      <c r="X30" s="29"/>
-      <c r="Y30" s="26"/>
-      <c r="Z30" s="26"/>
-      <c r="AA30" s="26"/>
+      <c r="S30" s="33"/>
+      <c r="T30" s="33"/>
+      <c r="U30" s="33"/>
+      <c r="V30" s="33"/>
+      <c r="W30" s="34"/>
+      <c r="X30" s="42"/>
+      <c r="Y30" s="85"/>
+      <c r="Z30" s="85"/>
+      <c r="AA30" s="85"/>
       <c r="AB30" s="10"/>
     </row>
     <row r="31" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>7</v>
       </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="27"/>
-      <c r="L31" s="27"/>
-      <c r="M31" s="27"/>
-      <c r="N31" s="27"/>
-      <c r="O31" s="27"/>
-      <c r="P31" s="27"/>
-      <c r="Q31" s="27"/>
+      <c r="B31" s="85"/>
+      <c r="C31" s="85"/>
+      <c r="D31" s="85"/>
+      <c r="E31" s="85"/>
+      <c r="F31" s="85"/>
+      <c r="G31" s="85"/>
+      <c r="H31" s="85"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="33"/>
+      <c r="M31" s="33"/>
+      <c r="N31" s="33"/>
+      <c r="O31" s="33"/>
+      <c r="P31" s="33"/>
+      <c r="Q31" s="33"/>
       <c r="R31" s="8"/>
-      <c r="S31" s="27"/>
-      <c r="T31" s="27"/>
-      <c r="U31" s="27"/>
-      <c r="V31" s="27"/>
-      <c r="W31" s="28"/>
-      <c r="X31" s="29"/>
-      <c r="Y31" s="26"/>
-      <c r="Z31" s="26"/>
-      <c r="AA31" s="26"/>
+      <c r="S31" s="33"/>
+      <c r="T31" s="33"/>
+      <c r="U31" s="33"/>
+      <c r="V31" s="33"/>
+      <c r="W31" s="34"/>
+      <c r="X31" s="42"/>
+      <c r="Y31" s="85"/>
+      <c r="Z31" s="85"/>
+      <c r="AA31" s="85"/>
       <c r="AB31" s="10"/>
     </row>
     <row r="32" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>8</v>
       </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="27"/>
-      <c r="L32" s="27"/>
-      <c r="M32" s="27"/>
-      <c r="N32" s="27"/>
-      <c r="O32" s="27"/>
-      <c r="P32" s="27"/>
-      <c r="Q32" s="27"/>
+      <c r="B32" s="85"/>
+      <c r="C32" s="85"/>
+      <c r="D32" s="85"/>
+      <c r="E32" s="85"/>
+      <c r="F32" s="85"/>
+      <c r="G32" s="85"/>
+      <c r="H32" s="85"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="33"/>
+      <c r="N32" s="33"/>
+      <c r="O32" s="33"/>
+      <c r="P32" s="33"/>
+      <c r="Q32" s="33"/>
       <c r="R32" s="8"/>
-      <c r="S32" s="27"/>
-      <c r="T32" s="27"/>
-      <c r="U32" s="27"/>
-      <c r="V32" s="27"/>
-      <c r="W32" s="28"/>
-      <c r="X32" s="29"/>
-      <c r="Y32" s="26"/>
-      <c r="Z32" s="26"/>
-      <c r="AA32" s="26"/>
+      <c r="S32" s="33"/>
+      <c r="T32" s="33"/>
+      <c r="U32" s="33"/>
+      <c r="V32" s="33"/>
+      <c r="W32" s="34"/>
+      <c r="X32" s="42"/>
+      <c r="Y32" s="85"/>
+      <c r="Z32" s="85"/>
+      <c r="AA32" s="85"/>
       <c r="AB32" s="10"/>
     </row>
     <row r="33" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>9</v>
       </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
-      <c r="L33" s="27"/>
-      <c r="M33" s="27"/>
-      <c r="N33" s="27"/>
-      <c r="O33" s="27"/>
-      <c r="P33" s="27"/>
-      <c r="Q33" s="27"/>
+      <c r="B33" s="85"/>
+      <c r="C33" s="85"/>
+      <c r="D33" s="85"/>
+      <c r="E33" s="85"/>
+      <c r="F33" s="85"/>
+      <c r="G33" s="85"/>
+      <c r="H33" s="85"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="33"/>
+      <c r="N33" s="33"/>
+      <c r="O33" s="33"/>
+      <c r="P33" s="33"/>
+      <c r="Q33" s="33"/>
       <c r="R33" s="8"/>
-      <c r="S33" s="27"/>
-      <c r="T33" s="27"/>
-      <c r="U33" s="27"/>
-      <c r="V33" s="27"/>
-      <c r="W33" s="28"/>
-      <c r="X33" s="29"/>
-      <c r="Y33" s="26"/>
-      <c r="Z33" s="26"/>
-      <c r="AA33" s="26"/>
+      <c r="S33" s="33"/>
+      <c r="T33" s="33"/>
+      <c r="U33" s="33"/>
+      <c r="V33" s="33"/>
+      <c r="W33" s="34"/>
+      <c r="X33" s="42"/>
+      <c r="Y33" s="85"/>
+      <c r="Z33" s="85"/>
+      <c r="AA33" s="85"/>
       <c r="AB33" s="10"/>
     </row>
     <row r="34" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
         <v>10</v>
       </c>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="27"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="27"/>
-      <c r="L34" s="27"/>
-      <c r="M34" s="27"/>
-      <c r="N34" s="27"/>
-      <c r="O34" s="27"/>
-      <c r="P34" s="27"/>
-      <c r="Q34" s="27"/>
+      <c r="B34" s="85"/>
+      <c r="C34" s="85"/>
+      <c r="D34" s="85"/>
+      <c r="E34" s="85"/>
+      <c r="F34" s="85"/>
+      <c r="G34" s="85"/>
+      <c r="H34" s="85"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="33"/>
+      <c r="K34" s="33"/>
+      <c r="L34" s="33"/>
+      <c r="M34" s="33"/>
+      <c r="N34" s="33"/>
+      <c r="O34" s="33"/>
+      <c r="P34" s="33"/>
+      <c r="Q34" s="33"/>
       <c r="R34" s="8"/>
-      <c r="S34" s="27"/>
-      <c r="T34" s="27"/>
-      <c r="U34" s="27"/>
-      <c r="V34" s="27"/>
-      <c r="W34" s="28"/>
-      <c r="X34" s="29"/>
-      <c r="Y34" s="26"/>
-      <c r="Z34" s="26"/>
-      <c r="AA34" s="26"/>
+      <c r="S34" s="33"/>
+      <c r="T34" s="33"/>
+      <c r="U34" s="33"/>
+      <c r="V34" s="33"/>
+      <c r="W34" s="34"/>
+      <c r="X34" s="42"/>
+      <c r="Y34" s="85"/>
+      <c r="Z34" s="85"/>
+      <c r="AA34" s="85"/>
       <c r="AB34" s="10"/>
     </row>
     <row r="35" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
         <v>11</v>
       </c>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="27"/>
-      <c r="K35" s="27"/>
-      <c r="L35" s="27"/>
-      <c r="M35" s="27"/>
-      <c r="N35" s="27"/>
-      <c r="O35" s="27"/>
-      <c r="P35" s="27"/>
-      <c r="Q35" s="27"/>
+      <c r="B35" s="85"/>
+      <c r="C35" s="85"/>
+      <c r="D35" s="85"/>
+      <c r="E35" s="85"/>
+      <c r="F35" s="85"/>
+      <c r="G35" s="85"/>
+      <c r="H35" s="85"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="33"/>
+      <c r="K35" s="33"/>
+      <c r="L35" s="33"/>
+      <c r="M35" s="33"/>
+      <c r="N35" s="33"/>
+      <c r="O35" s="33"/>
+      <c r="P35" s="33"/>
+      <c r="Q35" s="33"/>
       <c r="R35" s="8"/>
-      <c r="S35" s="27"/>
-      <c r="T35" s="27"/>
-      <c r="U35" s="27"/>
-      <c r="V35" s="27"/>
-      <c r="W35" s="28"/>
-      <c r="X35" s="29"/>
-      <c r="Y35" s="26"/>
-      <c r="Z35" s="26"/>
-      <c r="AA35" s="26"/>
+      <c r="S35" s="33"/>
+      <c r="T35" s="33"/>
+      <c r="U35" s="33"/>
+      <c r="V35" s="33"/>
+      <c r="W35" s="34"/>
+      <c r="X35" s="42"/>
+      <c r="Y35" s="85"/>
+      <c r="Z35" s="85"/>
+      <c r="AA35" s="85"/>
       <c r="AB35" s="10"/>
     </row>
     <row r="36" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>12</v>
       </c>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
-      <c r="I36" s="27"/>
-      <c r="J36" s="27"/>
-      <c r="K36" s="27"/>
-      <c r="L36" s="27"/>
-      <c r="M36" s="27"/>
-      <c r="N36" s="27"/>
-      <c r="O36" s="27"/>
-      <c r="P36" s="27"/>
-      <c r="Q36" s="27"/>
+      <c r="B36" s="85"/>
+      <c r="C36" s="85"/>
+      <c r="D36" s="85"/>
+      <c r="E36" s="85"/>
+      <c r="F36" s="85"/>
+      <c r="G36" s="85"/>
+      <c r="H36" s="85"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="33"/>
+      <c r="K36" s="33"/>
+      <c r="L36" s="33"/>
+      <c r="M36" s="33"/>
+      <c r="N36" s="33"/>
+      <c r="O36" s="33"/>
+      <c r="P36" s="33"/>
+      <c r="Q36" s="33"/>
       <c r="R36" s="8"/>
-      <c r="S36" s="27"/>
-      <c r="T36" s="27"/>
-      <c r="U36" s="27"/>
-      <c r="V36" s="27"/>
-      <c r="W36" s="28"/>
-      <c r="X36" s="29"/>
-      <c r="Y36" s="26"/>
-      <c r="Z36" s="26"/>
-      <c r="AA36" s="26"/>
+      <c r="S36" s="33"/>
+      <c r="T36" s="33"/>
+      <c r="U36" s="33"/>
+      <c r="V36" s="33"/>
+      <c r="W36" s="34"/>
+      <c r="X36" s="42"/>
+      <c r="Y36" s="85"/>
+      <c r="Z36" s="85"/>
+      <c r="AA36" s="85"/>
       <c r="AB36" s="10"/>
     </row>
     <row r="37" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>13</v>
       </c>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26"/>
-      <c r="I37" s="27"/>
-      <c r="J37" s="27"/>
-      <c r="K37" s="27"/>
-      <c r="L37" s="27"/>
-      <c r="M37" s="27"/>
-      <c r="N37" s="27"/>
-      <c r="O37" s="27"/>
-      <c r="P37" s="27"/>
-      <c r="Q37" s="27"/>
+      <c r="B37" s="85"/>
+      <c r="C37" s="85"/>
+      <c r="D37" s="85"/>
+      <c r="E37" s="85"/>
+      <c r="F37" s="85"/>
+      <c r="G37" s="85"/>
+      <c r="H37" s="85"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="33"/>
+      <c r="K37" s="33"/>
+      <c r="L37" s="33"/>
+      <c r="M37" s="33"/>
+      <c r="N37" s="33"/>
+      <c r="O37" s="33"/>
+      <c r="P37" s="33"/>
+      <c r="Q37" s="33"/>
       <c r="R37" s="8"/>
-      <c r="S37" s="27"/>
-      <c r="T37" s="27"/>
-      <c r="U37" s="27"/>
-      <c r="V37" s="27"/>
-      <c r="W37" s="28"/>
-      <c r="X37" s="29"/>
-      <c r="Y37" s="26"/>
-      <c r="Z37" s="26"/>
-      <c r="AA37" s="26"/>
+      <c r="S37" s="33"/>
+      <c r="T37" s="33"/>
+      <c r="U37" s="33"/>
+      <c r="V37" s="33"/>
+      <c r="W37" s="34"/>
+      <c r="X37" s="42"/>
+      <c r="Y37" s="85"/>
+      <c r="Z37" s="85"/>
+      <c r="AA37" s="85"/>
       <c r="AB37" s="10"/>
     </row>
     <row r="38" spans="1:28" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11">
         <v>14</v>
       </c>
-      <c r="B38" s="55"/>
-      <c r="C38" s="55"/>
-      <c r="D38" s="55"/>
-      <c r="E38" s="55"/>
-      <c r="F38" s="55"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="44"/>
-      <c r="J38" s="44"/>
-      <c r="K38" s="44"/>
-      <c r="L38" s="44"/>
-      <c r="M38" s="44"/>
-      <c r="N38" s="44"/>
-      <c r="O38" s="44"/>
-      <c r="P38" s="44"/>
-      <c r="Q38" s="44"/>
+      <c r="B38" s="83"/>
+      <c r="C38" s="83"/>
+      <c r="D38" s="83"/>
+      <c r="E38" s="83"/>
+      <c r="F38" s="83"/>
+      <c r="G38" s="83"/>
+      <c r="H38" s="83"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="38"/>
+      <c r="K38" s="38"/>
+      <c r="L38" s="38"/>
+      <c r="M38" s="38"/>
+      <c r="N38" s="38"/>
+      <c r="O38" s="38"/>
+      <c r="P38" s="38"/>
+      <c r="Q38" s="38"/>
       <c r="R38" s="12"/>
-      <c r="S38" s="44"/>
-      <c r="T38" s="44"/>
-      <c r="U38" s="44"/>
-      <c r="V38" s="44"/>
-      <c r="W38" s="56"/>
-      <c r="X38" s="57"/>
-      <c r="Y38" s="55"/>
-      <c r="Z38" s="55"/>
-      <c r="AA38" s="55"/>
+      <c r="S38" s="38"/>
+      <c r="T38" s="38"/>
+      <c r="U38" s="38"/>
+      <c r="V38" s="38"/>
+      <c r="W38" s="39"/>
+      <c r="X38" s="86"/>
+      <c r="Y38" s="83"/>
+      <c r="Z38" s="83"/>
+      <c r="AA38" s="83"/>
       <c r="AB38" s="13"/>
     </row>
     <row r="39" spans="1:28" s="3" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="49" t="s">
+      <c r="A39" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="B39" s="50"/>
-      <c r="C39" s="50"/>
-      <c r="D39" s="50"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="51" t="s">
+      <c r="B39" s="89"/>
+      <c r="C39" s="89"/>
+      <c r="D39" s="89"/>
+      <c r="E39" s="89"/>
+      <c r="F39" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="G39" s="51"/>
-      <c r="H39" s="51"/>
-      <c r="I39" s="51"/>
-      <c r="J39" s="51"/>
-      <c r="K39" s="51"/>
-      <c r="L39" s="51"/>
-      <c r="M39" s="51"/>
-      <c r="N39" s="51"/>
-      <c r="O39" s="51"/>
-      <c r="P39" s="52" t="s">
+      <c r="G39" s="90"/>
+      <c r="H39" s="90"/>
+      <c r="I39" s="90"/>
+      <c r="J39" s="90"/>
+      <c r="K39" s="90"/>
+      <c r="L39" s="90"/>
+      <c r="M39" s="90"/>
+      <c r="N39" s="90"/>
+      <c r="O39" s="90"/>
+      <c r="P39" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="Q39" s="52"/>
-      <c r="R39" s="52"/>
-      <c r="S39" s="52"/>
-      <c r="T39" s="52"/>
-      <c r="U39" s="52" t="s">
+      <c r="Q39" s="66"/>
+      <c r="R39" s="66"/>
+      <c r="S39" s="66"/>
+      <c r="T39" s="66"/>
+      <c r="U39" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="V39" s="52"/>
-      <c r="W39" s="52"/>
-      <c r="X39" s="52"/>
-      <c r="Y39" s="52"/>
-      <c r="Z39" s="52" t="s">
+      <c r="V39" s="66"/>
+      <c r="W39" s="66"/>
+      <c r="X39" s="66"/>
+      <c r="Y39" s="66"/>
+      <c r="Z39" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="AA39" s="52"/>
-      <c r="AB39" s="53"/>
+      <c r="AA39" s="66"/>
+      <c r="AB39" s="67"/>
     </row>
     <row r="40" spans="1:28" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="46" t="s">
+      <c r="A40" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="47"/>
-      <c r="C40" s="47"/>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="27"/>
-      <c r="I40" s="27"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="27"/>
-      <c r="L40" s="27"/>
-      <c r="M40" s="27"/>
-      <c r="N40" s="27"/>
-      <c r="O40" s="27"/>
-      <c r="P40" s="28"/>
-      <c r="Q40" s="54"/>
-      <c r="R40" s="54"/>
-      <c r="S40" s="54"/>
-      <c r="T40" s="29"/>
-      <c r="U40" s="28"/>
-      <c r="V40" s="54"/>
-      <c r="W40" s="54"/>
-      <c r="X40" s="54"/>
-      <c r="Y40" s="29"/>
-      <c r="Z40" s="27"/>
-      <c r="AA40" s="27"/>
-      <c r="AB40" s="48"/>
+      <c r="B40" s="92"/>
+      <c r="C40" s="92"/>
+      <c r="D40" s="92"/>
+      <c r="E40" s="92"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="33"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="33"/>
+      <c r="L40" s="33"/>
+      <c r="M40" s="33"/>
+      <c r="N40" s="33"/>
+      <c r="O40" s="33"/>
+      <c r="P40" s="34"/>
+      <c r="Q40" s="41"/>
+      <c r="R40" s="41"/>
+      <c r="S40" s="41"/>
+      <c r="T40" s="42"/>
+      <c r="U40" s="34"/>
+      <c r="V40" s="41"/>
+      <c r="W40" s="41"/>
+      <c r="X40" s="41"/>
+      <c r="Y40" s="42"/>
+      <c r="Z40" s="33"/>
+      <c r="AA40" s="33"/>
+      <c r="AB40" s="87"/>
     </row>
     <row r="41" spans="1:28" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="46" t="s">
+      <c r="A41" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="B41" s="47"/>
-      <c r="C41" s="47"/>
-      <c r="D41" s="47"/>
-      <c r="E41" s="47"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="27"/>
-      <c r="H41" s="27"/>
-      <c r="I41" s="27"/>
-      <c r="J41" s="27"/>
-      <c r="K41" s="27"/>
-      <c r="L41" s="27"/>
-      <c r="M41" s="27"/>
-      <c r="N41" s="27"/>
-      <c r="O41" s="27"/>
-      <c r="P41" s="27"/>
-      <c r="Q41" s="27"/>
-      <c r="R41" s="27"/>
-      <c r="S41" s="27"/>
-      <c r="T41" s="27"/>
-      <c r="U41" s="27"/>
-      <c r="V41" s="27"/>
-      <c r="W41" s="27"/>
-      <c r="X41" s="27"/>
-      <c r="Y41" s="27"/>
-      <c r="Z41" s="27"/>
-      <c r="AA41" s="27"/>
-      <c r="AB41" s="48"/>
+      <c r="B41" s="92"/>
+      <c r="C41" s="92"/>
+      <c r="D41" s="92"/>
+      <c r="E41" s="92"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="33"/>
+      <c r="I41" s="33"/>
+      <c r="J41" s="33"/>
+      <c r="K41" s="33"/>
+      <c r="L41" s="33"/>
+      <c r="M41" s="33"/>
+      <c r="N41" s="33"/>
+      <c r="O41" s="33"/>
+      <c r="P41" s="33"/>
+      <c r="Q41" s="33"/>
+      <c r="R41" s="33"/>
+      <c r="S41" s="33"/>
+      <c r="T41" s="33"/>
+      <c r="U41" s="33"/>
+      <c r="V41" s="33"/>
+      <c r="W41" s="33"/>
+      <c r="X41" s="33"/>
+      <c r="Y41" s="33"/>
+      <c r="Z41" s="33"/>
+      <c r="AA41" s="33"/>
+      <c r="AB41" s="87"/>
     </row>
     <row r="42" spans="1:28" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="B42" s="47"/>
-      <c r="C42" s="47"/>
-      <c r="D42" s="47"/>
-      <c r="E42" s="47"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="27"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="27"/>
-      <c r="J42" s="27"/>
-      <c r="K42" s="27"/>
-      <c r="L42" s="27"/>
-      <c r="M42" s="27"/>
-      <c r="N42" s="27"/>
-      <c r="O42" s="27"/>
-      <c r="P42" s="27"/>
-      <c r="Q42" s="27"/>
-      <c r="R42" s="27"/>
-      <c r="S42" s="27"/>
-      <c r="T42" s="27"/>
-      <c r="U42" s="27"/>
-      <c r="V42" s="27"/>
-      <c r="W42" s="27"/>
-      <c r="X42" s="27"/>
-      <c r="Y42" s="27"/>
-      <c r="Z42" s="27"/>
-      <c r="AA42" s="27"/>
-      <c r="AB42" s="48"/>
+      <c r="B42" s="92"/>
+      <c r="C42" s="92"/>
+      <c r="D42" s="92"/>
+      <c r="E42" s="92"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="33"/>
+      <c r="H42" s="33"/>
+      <c r="I42" s="33"/>
+      <c r="J42" s="33"/>
+      <c r="K42" s="33"/>
+      <c r="L42" s="33"/>
+      <c r="M42" s="33"/>
+      <c r="N42" s="33"/>
+      <c r="O42" s="33"/>
+      <c r="P42" s="33"/>
+      <c r="Q42" s="33"/>
+      <c r="R42" s="33"/>
+      <c r="S42" s="33"/>
+      <c r="T42" s="33"/>
+      <c r="U42" s="33"/>
+      <c r="V42" s="33"/>
+      <c r="W42" s="33"/>
+      <c r="X42" s="33"/>
+      <c r="Y42" s="33"/>
+      <c r="Z42" s="33"/>
+      <c r="AA42" s="33"/>
+      <c r="AB42" s="87"/>
     </row>
     <row r="43" spans="1:28" ht="57.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="42" t="s">
+      <c r="A43" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="B43" s="43"/>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="44"/>
-      <c r="G43" s="44"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="44"/>
-      <c r="K43" s="44"/>
-      <c r="L43" s="44"/>
-      <c r="M43" s="44"/>
-      <c r="N43" s="44"/>
-      <c r="O43" s="44"/>
-      <c r="P43" s="44"/>
-      <c r="Q43" s="44"/>
-      <c r="R43" s="44"/>
-      <c r="S43" s="44"/>
-      <c r="T43" s="44"/>
-      <c r="U43" s="44"/>
-      <c r="V43" s="44"/>
-      <c r="W43" s="44"/>
-      <c r="X43" s="44"/>
-      <c r="Y43" s="44"/>
-      <c r="Z43" s="44"/>
-      <c r="AA43" s="44"/>
-      <c r="AB43" s="45"/>
+      <c r="B43" s="96"/>
+      <c r="C43" s="96"/>
+      <c r="D43" s="96"/>
+      <c r="E43" s="96"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="38"/>
+      <c r="K43" s="38"/>
+      <c r="L43" s="38"/>
+      <c r="M43" s="38"/>
+      <c r="N43" s="38"/>
+      <c r="O43" s="38"/>
+      <c r="P43" s="38"/>
+      <c r="Q43" s="38"/>
+      <c r="R43" s="38"/>
+      <c r="S43" s="38"/>
+      <c r="T43" s="38"/>
+      <c r="U43" s="38"/>
+      <c r="V43" s="38"/>
+      <c r="W43" s="38"/>
+      <c r="X43" s="38"/>
+      <c r="Y43" s="38"/>
+      <c r="Z43" s="38"/>
+      <c r="AA43" s="38"/>
+      <c r="AB43" s="97"/>
     </row>
     <row r="44" spans="1:28" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="B44" s="39"/>
-      <c r="C44" s="39"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="39"/>
-      <c r="J44" s="39"/>
-      <c r="K44" s="39"/>
-      <c r="L44" s="39"/>
-      <c r="M44" s="39"/>
-      <c r="N44" s="39"/>
-      <c r="O44" s="39"/>
-      <c r="P44" s="39"/>
-      <c r="Q44" s="39"/>
-      <c r="R44" s="39"/>
-      <c r="S44" s="39"/>
-      <c r="T44" s="39"/>
-      <c r="U44" s="39"/>
-      <c r="V44" s="39"/>
-      <c r="W44" s="39"/>
-      <c r="X44" s="39"/>
-      <c r="Y44" s="39"/>
-      <c r="Z44" s="39"/>
-      <c r="AA44" s="39"/>
-      <c r="AB44" s="39"/>
+      <c r="A44" s="93"/>
+      <c r="B44" s="94"/>
+      <c r="C44" s="94"/>
+      <c r="D44" s="94"/>
+      <c r="E44" s="94"/>
+      <c r="F44" s="94"/>
+      <c r="G44" s="94"/>
+      <c r="H44" s="94"/>
+      <c r="I44" s="94"/>
+      <c r="J44" s="94"/>
+      <c r="K44" s="94"/>
+      <c r="L44" s="94"/>
+      <c r="M44" s="94"/>
+      <c r="N44" s="94"/>
+      <c r="O44" s="94"/>
+      <c r="P44" s="94"/>
+      <c r="Q44" s="94"/>
+      <c r="R44" s="94"/>
+      <c r="S44" s="94"/>
+      <c r="T44" s="94"/>
+      <c r="U44" s="94"/>
+      <c r="V44" s="94"/>
+      <c r="W44" s="94"/>
+      <c r="X44" s="94"/>
+      <c r="Y44" s="94"/>
+      <c r="Z44" s="94"/>
+      <c r="AA44" s="94"/>
+      <c r="AB44" s="94"/>
     </row>
     <row r="45" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4545,89 +4581,101 @@
     <row r="429" ht="2.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="202">
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="H1:AB1"/>
-    <mergeCell ref="H2:AB2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:P3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="T3:W3"/>
-    <mergeCell ref="X3:Z3"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:P5"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="X5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:P4"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="T4:W4"/>
-    <mergeCell ref="X4:Z4"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:P7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="T7:W7"/>
-    <mergeCell ref="X7:Z7"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:P6"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="T6:W6"/>
-    <mergeCell ref="X6:Z6"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="E11:J11"/>
-    <mergeCell ref="K11:P11"/>
-    <mergeCell ref="Q11:V11"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="K10:P10"/>
-    <mergeCell ref="Q10:V10"/>
-    <mergeCell ref="A8:AB8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="K9:P9"/>
-    <mergeCell ref="Q9:V9"/>
-    <mergeCell ref="W9:Y9"/>
-    <mergeCell ref="Z9:AB9"/>
-    <mergeCell ref="S18:AB18"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="S19:AB19"/>
-    <mergeCell ref="A15:G19"/>
-    <mergeCell ref="H15:P19"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="S16:AB16"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="S17:AB17"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="Q15:AB15"/>
-    <mergeCell ref="A23:AB23"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="L24:Q24"/>
-    <mergeCell ref="S24:V24"/>
-    <mergeCell ref="W24:X24"/>
-    <mergeCell ref="Y24:AA24"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="H20:AB20"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="H21:AB21"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="H22:AB22"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="L26:Q26"/>
-    <mergeCell ref="S26:V26"/>
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="Y26:AA26"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="L25:Q25"/>
-    <mergeCell ref="S25:V25"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="Y25:AA25"/>
+    <mergeCell ref="W13:Y13"/>
+    <mergeCell ref="W14:Y14"/>
+    <mergeCell ref="Z13:AB13"/>
+    <mergeCell ref="Z14:AB14"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="L32:Q32"/>
+    <mergeCell ref="S32:V32"/>
+    <mergeCell ref="W32:X32"/>
+    <mergeCell ref="Y32:AA32"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="L31:Q31"/>
+    <mergeCell ref="S31:V31"/>
+    <mergeCell ref="W31:X31"/>
+    <mergeCell ref="Y31:AA31"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="L30:Q30"/>
+    <mergeCell ref="S30:V30"/>
+    <mergeCell ref="W30:X30"/>
+    <mergeCell ref="Y30:AA30"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="L29:Q29"/>
+    <mergeCell ref="S29:V29"/>
+    <mergeCell ref="W29:X29"/>
+    <mergeCell ref="Y29:AA29"/>
+    <mergeCell ref="Z12:AB12"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="L28:Q28"/>
+    <mergeCell ref="S28:V28"/>
+    <mergeCell ref="W28:X28"/>
+    <mergeCell ref="Y28:AA28"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="E14:J14"/>
+    <mergeCell ref="K14:P14"/>
+    <mergeCell ref="Q14:V14"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="E12:J12"/>
+    <mergeCell ref="K12:P12"/>
+    <mergeCell ref="Q12:V12"/>
+    <mergeCell ref="W12:Y12"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="L27:Q27"/>
+    <mergeCell ref="S27:V27"/>
+    <mergeCell ref="W27:X27"/>
+    <mergeCell ref="Y27:AA27"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="A44:AB44"/>
+    <mergeCell ref="W10:Y11"/>
+    <mergeCell ref="Z10:AB11"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="E13:J13"/>
+    <mergeCell ref="K13:P13"/>
+    <mergeCell ref="Q13:V13"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="F43:O43"/>
+    <mergeCell ref="P43:T43"/>
+    <mergeCell ref="U43:Y43"/>
+    <mergeCell ref="Z43:AB43"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="F41:O41"/>
+    <mergeCell ref="P41:T41"/>
+    <mergeCell ref="U41:Y41"/>
+    <mergeCell ref="Z41:AB41"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="F42:O42"/>
+    <mergeCell ref="P42:T42"/>
+    <mergeCell ref="U42:Y42"/>
+    <mergeCell ref="Z42:AB42"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="F39:O39"/>
+    <mergeCell ref="P39:T39"/>
+    <mergeCell ref="U39:Y39"/>
+    <mergeCell ref="Z39:AB39"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="F40:O40"/>
+    <mergeCell ref="P40:T40"/>
+    <mergeCell ref="U40:Y40"/>
+    <mergeCell ref="Z40:AB40"/>
+    <mergeCell ref="B38:H38"/>
+    <mergeCell ref="I38:K38"/>
+    <mergeCell ref="L38:Q38"/>
+    <mergeCell ref="S38:V38"/>
+    <mergeCell ref="W38:X38"/>
+    <mergeCell ref="Y38:AA38"/>
+    <mergeCell ref="B37:H37"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="L37:Q37"/>
+    <mergeCell ref="S37:V37"/>
+    <mergeCell ref="W37:X37"/>
+    <mergeCell ref="Y37:AA37"/>
     <mergeCell ref="B36:H36"/>
     <mergeCell ref="I36:K36"/>
     <mergeCell ref="L36:Q36"/>
@@ -4652,105 +4700,144 @@
     <mergeCell ref="S34:V34"/>
     <mergeCell ref="W34:X34"/>
     <mergeCell ref="Y34:AA34"/>
-    <mergeCell ref="B38:H38"/>
-    <mergeCell ref="I38:K38"/>
-    <mergeCell ref="L38:Q38"/>
-    <mergeCell ref="S38:V38"/>
-    <mergeCell ref="W38:X38"/>
-    <mergeCell ref="Y38:AA38"/>
-    <mergeCell ref="B37:H37"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="L37:Q37"/>
-    <mergeCell ref="S37:V37"/>
-    <mergeCell ref="W37:X37"/>
-    <mergeCell ref="Y37:AA37"/>
-    <mergeCell ref="Z42:AB42"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="F39:O39"/>
-    <mergeCell ref="P39:T39"/>
-    <mergeCell ref="U39:Y39"/>
-    <mergeCell ref="Z39:AB39"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="F40:O40"/>
-    <mergeCell ref="P40:T40"/>
-    <mergeCell ref="U40:Y40"/>
-    <mergeCell ref="Z40:AB40"/>
-    <mergeCell ref="W27:X27"/>
-    <mergeCell ref="Y27:AA27"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="A44:AB44"/>
-    <mergeCell ref="W10:Y11"/>
-    <mergeCell ref="Z10:AB11"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="E13:J13"/>
-    <mergeCell ref="K13:P13"/>
-    <mergeCell ref="Q13:V13"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="F43:O43"/>
-    <mergeCell ref="P43:T43"/>
-    <mergeCell ref="U43:Y43"/>
-    <mergeCell ref="Z43:AB43"/>
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="F41:O41"/>
-    <mergeCell ref="P41:T41"/>
-    <mergeCell ref="U41:Y41"/>
-    <mergeCell ref="Z41:AB41"/>
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="F42:O42"/>
-    <mergeCell ref="P42:T42"/>
-    <mergeCell ref="U42:Y42"/>
-    <mergeCell ref="L29:Q29"/>
-    <mergeCell ref="S29:V29"/>
-    <mergeCell ref="W29:X29"/>
-    <mergeCell ref="Y29:AA29"/>
-    <mergeCell ref="Z12:AB12"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="L28:Q28"/>
-    <mergeCell ref="S28:V28"/>
-    <mergeCell ref="W28:X28"/>
-    <mergeCell ref="Y28:AA28"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="E14:J14"/>
-    <mergeCell ref="K14:P14"/>
-    <mergeCell ref="Q14:V14"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="E12:J12"/>
-    <mergeCell ref="K12:P12"/>
-    <mergeCell ref="Q12:V12"/>
-    <mergeCell ref="W12:Y12"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="L27:Q27"/>
-    <mergeCell ref="S27:V27"/>
-    <mergeCell ref="W13:Y13"/>
-    <mergeCell ref="W14:Y14"/>
-    <mergeCell ref="Z13:AB13"/>
-    <mergeCell ref="Z14:AB14"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="L32:Q32"/>
-    <mergeCell ref="S32:V32"/>
-    <mergeCell ref="W32:X32"/>
-    <mergeCell ref="Y32:AA32"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="L31:Q31"/>
-    <mergeCell ref="S31:V31"/>
-    <mergeCell ref="W31:X31"/>
-    <mergeCell ref="Y31:AA31"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="L30:Q30"/>
-    <mergeCell ref="S30:V30"/>
-    <mergeCell ref="W30:X30"/>
-    <mergeCell ref="Y30:AA30"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="L26:Q26"/>
+    <mergeCell ref="S26:V26"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="Y26:AA26"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="L25:Q25"/>
+    <mergeCell ref="S25:V25"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="Y25:AA25"/>
+    <mergeCell ref="A23:AB23"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="L24:Q24"/>
+    <mergeCell ref="S24:V24"/>
+    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="Y24:AA24"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="H20:AB20"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="H21:AB21"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="H22:AB22"/>
+    <mergeCell ref="S18:AB18"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="S19:AB19"/>
+    <mergeCell ref="A15:G19"/>
+    <mergeCell ref="H15:P19"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="S16:AB16"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="S17:AB17"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="Q15:AB15"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="E11:J11"/>
+    <mergeCell ref="K11:P11"/>
+    <mergeCell ref="Q11:V11"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="K10:P10"/>
+    <mergeCell ref="Q10:V10"/>
+    <mergeCell ref="A8:AB8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="K9:P9"/>
+    <mergeCell ref="Q9:V9"/>
+    <mergeCell ref="W9:Y9"/>
+    <mergeCell ref="Z9:AB9"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:P7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="T7:W7"/>
+    <mergeCell ref="X7:Z7"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:P6"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="T6:W6"/>
+    <mergeCell ref="X6:Z6"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:P5"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="X5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:P4"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="T4:W4"/>
+    <mergeCell ref="X4:Z4"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="H1:AB1"/>
+    <mergeCell ref="H2:AB2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="T3:W3"/>
+    <mergeCell ref="X3:Z3"/>
+    <mergeCell ref="AA3:AB3"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157499" right="0" top="0.27558836395450598" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="72" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1025" r:id="rId4" name="Check Box 1">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>274320</xdr:colOff>
+                    <xdr:row>17</xdr:row>
+                    <xdr:rowOff>83820</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>190500</xdr:colOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>53340</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1026" r:id="rId5" name="Check Box 2">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>15</xdr:col>
+                    <xdr:colOff>160020</xdr:colOff>
+                    <xdr:row>17</xdr:row>
+                    <xdr:rowOff>91440</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>15</xdr:col>
+                    <xdr:colOff>487680</xdr:colOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>53340</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
</xml_diff>